<commit_message>
BMW_SecOc 0404 first edition
</commit_message>
<xml_diff>
--- a/BMW_SecOc.xlsx
+++ b/BMW_SecOc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git_XuhuaRepo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A35FE04-AF55-4D28-9128-AA7FE1F3041F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E84A7BCD-F8AA-4D08-9E92-F5C7F36ADA7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-8640" windowWidth="38640" windowHeight="21240" xr2:uid="{EE3554E5-5B85-4F6F-95D2-24E55C4E92D2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Part 1: Common part, regadless of its direction</t>
   </si>
@@ -36,45 +36,610 @@
     <t>Part 3: RX secured IPDU</t>
   </si>
   <si>
-    <t>DsBusCustomCode_onApplicationInitPrivate(pduFeatureHandle)</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <t>DsBusCustomCode_onPduFeatureExecutionPrivate(pduFeatureHandle)</t>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>DsBusCustomCode_onPduFeatureExecutionPrivate(pduFeatureHandle)</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>PduPropertiesContainer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> *</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>pduProps</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">
+{
+        //Properties for PDU Features general
+        DsBusCustomCodePduFeatureHandle PduFeatureHandle;
+        uint32 AuthType;
+        char *KeyAsString;
+        boolean IsTx;
+        boolean IsRx;
+        ClusterAgentStruct *ClusterAgent;
+        DsBusCustomCodeEcuHandle EcuHandle;
+        char *EcuName;
+        boolean IsCounterMessage;
+        boolean IsCounterResponseMessage;
+        boolean IsAnyCounterMessage;
+        boolean HasSlManipulationBlock;
+        boolean *FreshnessOverwriteEnable;
+        uint32 *FreshnessOverwriteValue;
+        boolean *AuthenticatorBytesOverwriteEnable[MAX_NUM_MAC_DATA_BYTES];
+        uint8 *AuthenticatorBytesOverwriteValue[MAX_NUM_MAC_DATA_BYTES];
+        //Properties for Secured PDU 
+        DsBusCustomCodePduHandle SecuredIPdu_PduHandle;
+        char *SecuredIPdu_Name;
+        uint8 *SecuredIPdu_SduDataPtr;
+        uint32 SecuredIPdu_SduLength;
+        uint16 SecuredIPdu_DataId;
+        uint32 SecuredIPdu_KeyId;
+        uint32 SecuredIPdu_AuthenticIPduPosition;
+        uint32 MacPosition; // = in Bits
+        uint32 MacTruncatedLength; // = AuthInfoTxLength = Length in Bits
+        uint32 FreshnessValuePosition; //Position in Bits
+        uint32 FreshnessValLength; // = Length in Bits
+        uint32 FreshnessValTruncatedLength; // = Length in Bits
+        boolean UseSecuredPduAsCryptoPduForMsgSplitUp;
+        uint32 SecuredIPdu_MessageLinkPosition;
+        uint16 MessageLinkPosition; // = Position in Bits
+        uint16 MessageLinkLength; // = Length in Bits
+        //int HasLimitedSecuredPayloadArea;
+        uint32 SecuredAreaOffset;
+        uint32 SecuredAreaLength; // = Length in Bytes
+        //Properties for Authentic PDU
+        DsBusCustomCodePduHandle AuthenticIPdu_PduHandle;
+        char *AuthenticIPdu_Name;
+        uint8 *AuthenticIPdu_SduDataPtr;
+        uint32 AuthenticIPdu_SduLength; // = Length in Bytes
+        uint32 AuthenticIPdu_ActualSduLength; // = Length in Bytes
+        uint8 AuthPduHeaderLength; // = Length in Bytes
+    } </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>PduPropertiesContainer</t>
+    </r>
   </si>
   <si>
-    <t>DsBusCustomCode_onApplicationInitPrivateUnhandled(pduFeatureHandle)</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>pduFeatData</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>-&gt;PduPropertiesContainer = (uint8*)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>pduProps</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
+    <t>DsBusCustomCode_onApplicationInitPrivate(pduFeatureHandle) / DsBusCustomCode_onApplicationInitPrivateUnhandled(pduFeatureHandle)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF00FF"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>ECU-Infos</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>pduProps</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">-&gt;EcuHandle = ecuHandle;
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>pduProps</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">-&gt;EcuName = ecuName;
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF00FF"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>Secured IPDU</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>pduProps</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">-&gt;SecuredIPdu_PduHandle = securedIPdu_PduHandle;
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>pduProps</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">-&gt;SecuredIPdu_Name = securedIPdu_Name;
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>pduProps</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">-&gt;IsTx = isTx;
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>pduProps</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">-&gt;IsRx = !isTx;
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>pduProps</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">-&gt;SecuredIPdu_SduLength = securedIPdu_SduLength
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>pduProps</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">-&gt;SecuredIPdu_DataId = dataId
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>pduProps</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">-&gt;MacTruncatedLength = authInfoTxLength
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>pduProps</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">-&gt;UseSecuredPduAsCryptoPduForMsgSplitUp = useAsCryptographicPdu;
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>pduProps</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">-&gt;MessageLinkLength = messageLinkLength;
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>pduProps</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">-&gt;MessageLinkPosition = messageLinkPosition;
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>pduProps</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">-&gt;AuthPduHeaderLength = authPduHeaderLength
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>pduProps</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">-&gt;SecuredIPdu_AuthenticIPduPosition = securedIPduAuthenticIPduPosition
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF00FF"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>Authentic PDU</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>pduProps</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">-&gt;AuthenticIPdu_PduHandle = authenticIPdu_PduHandle;
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>pduProps</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">-&gt;AuthenticIPdu_SduLength = authenticIPdu_SduLength;
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>pduProps</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>-&gt;AuthenticIPdu_Name = authenticIPdu_Name;</t>
+    </r>
+  </si>
+  <si>
+    <t>UserCode_FeatureData</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
       </rPr>
       <t>UserCode_FeatureData</t>
     </r>
     <r>
       <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> *pduFeatData
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> *</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>pduFeatData</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">
 pduFeatDataPtr = (uint8*)pduFeatData;
 DsBusCustomCodePduFeature_setFeatureDataPtr(pduFeatureHandle, pduFeatDataPtr)
 {
-    uint8 *PduPropertiesContainer;
+    uint8 *</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>PduPropertiesContainer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">;
     char* FeatureDescriptor;
     uint8* CsmJobHandle;
     uint8  IsInitialized; // Set to 1 if everything for the feature handle was set up
@@ -89,13 +654,190 @@
     <r>
       <rPr>
         <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>UserCode_FeatureData</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">;
+</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Assign the instantiated UserCode_FeatureData struct via its pduFeatData pointer to the featureDataPtr pointer.
+Assign the featureDataPtr pointer to the PDUFeatureHandle.
+</t>
+    </r>
+    <r>
+      <rPr>
         <i/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>Put UserCode pointer in DsPduFeatureHandle structure</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>DsBusCustomCode_collectStaticPduProperties(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>pduFeatData</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>)
+DsBusCustomCode_collectStaticPduPropertiesEx(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>pduFeatData</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">)
+_____________________________________________________________
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF00FF"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>Cluster-Infos</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">
+DsBusCustomCode_createClusterAgent(pduFeatData)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF00FF"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>ECU-Infos</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">
+GetPropertiesForEcu(pduProps-&gt;PduFeatureHandle, &amp;ecuHandle, &amp;ecuName)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF00FF"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>Secured IPDU</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">
+DsBusCustomCodePduFeature_getPdu(pduProps-&gt;PduFeatureHandle, &amp;securedIPdu_PduHandle)
+DsBusCustomCode_getName(securedIPdu_PduHandle, &amp;securedIPdu_Name)
+DsBusCustomCodePdu_getIsTx(securedIPdu_PduHandle, &amp;isTx)
+DsBusCustomCodePdu_getSduLength(securedIPdu_PduHandle, &amp;securedIPdu_SduLength)
+DsBusCustomCodeSecuredIPdu_getDataId(securedIPdu_PduHandle, &amp;dataId)
+DsBusCustomCodeSecuredIPdu_getAuthInfoTxLength(securedIPdu_PduHandle,&amp;authInfoTxLength)
+IdentifyPropertiesForSplitUpCryptoPdu(pduFeatData, &amp;useAsCryptographicPdu,&amp;messageLinkLength, &amp;messageLinkPosition)
+DsBusCustomCodeSecuredIPdu_getAuthPduHeaderLength(securedIPdu_PduHandle, &amp;authPduHeaderLength)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF00FF"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>Authentic PDU</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">
+DsBusCustomCodeSecuredIPdu_getAuthenticPdu(securedIPdu_PduHandle, &amp;authenticIPdu_PduHandle)
+DsBusCustomCodePdu_getSduLength(authenticIPdu_PduHandle, &amp;authenticIPdu_SduLength)
+DsBusCustomCode_getName(authenticIPdu_PduHandle, &amp;authenticIPdu_Name)</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">get </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
       </rPr>
       <t>UserCode_FeatureData</t>
     </r>
@@ -104,20 +846,1186 @@
         <i/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>pduFeatDataPtr</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> pointer set in pduFeatureHandle before to access the data</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>UserCode_Csm_Init(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>pduProps</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>-&gt;PduFeatureHandle)
+_____________________________________________________________
+DsBusCustomCodePduFeature_getFeatureDataPtr(pduFeatureHandle, &amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>pduFeatDataPtr</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>UserCode_FeatureData</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> *</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>pduFeatData</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> = (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>UserCode_FeatureData</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>*)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>pduFeatDataPtr</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">;
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>pduFeatData</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>-&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>CsmJobHandle</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> = NULL;
+</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>_UserCode_Csm_Init(DsBusCustomCodePduFeatureHandle pduFeatureHandle, boolean atRuntime), atRuntime = FALSE
+_____________________________________________________________
+DsBusCustomCodePduFeature_getFeatureDataPtr(pduFeatureHandle, &amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>pduFeatDataPtr</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>pduFeatData</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> = (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>UserCode_FeatureData</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>*)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>pduFeatDataPtr</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">; 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>pduProps</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> = (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>PduPropertiesContainer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>*)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>pduFeatData</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>-&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>PduPropertiesContainer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>;
+DsBusCustomCodeSecuredIPdu_getFreshnessValueLength(securedIPdu_PduHandle, &amp;freshnessValueLength)
+dataToAuthentictatorLenInBytes = sizeof(uint16) + authenticIPdu_SduLength + (freshnessValueLength + 7) / 8
+UserCode_SecOCHelper_Create_CryptoJob_For_CMAC_AES_128_Authentication(&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>pduFeatData</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>-&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>CsmJobHandle</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">,dataToAuthentictatorLenInBytes)
+_____________________________________________________________
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>Crypto_Job</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>UserCode_CryptoJob_Register(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>Crypto_Job</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>, &amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>csmJobHandle</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, &amp;jobIdInternal)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">
+*</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>CsmJobHandle</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>csmJobHandle</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>UserCode_CryptoJob_Register(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>Crypto_Job</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>, &amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>csmJobHandle</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, &amp;jobIdInternal)
+_______________________________
+{
+    struct </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="9" tint="-0.499984740745262"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>AES_ctx</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">* </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="9" tint="-0.499984740745262"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>CTX_Handle</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">;
+    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>Crypto_JobType</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">* </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>Crypto_Job</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">;
+} </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>CsmJobHandle_Type</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">;
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>CsmJobHandle_Type</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">* </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>jobHandle</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> = (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>CsmJobHandle_Type</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>*)rtlib_malloc(sizeof(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>CsmJobHandle_Type</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">))
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>jobHandle</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>-&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">Crypto_Job </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">= </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>Crypto_Job</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">
+*</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>CsmJobHandle</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> = (uint8*) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">jobHandle
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>Note:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">CsmJobHandle </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">is </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>CsmJobHandle_Type</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>UserCode_Csm_KeyElementInit(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>pduFeatData</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>-&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>CsmJobHandle</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, CRYPTO_KE_MAC_KEY), CRYPTO_KE_MAC_KEY = 0x01
+_____________________________________________________________
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>CsmJobHandle_Type</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">* </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>jobHandle</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> = (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>CsmJobHandle_Type</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>*)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>CsmJobHandle</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">
+struct </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="9" tint="-0.499984740745262"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>AES_ctx</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">* </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>handle</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> = Ds_CMAC_New();
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>jobHandle</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>-&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="9" tint="-0.499984740745262"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>CTX_Handle</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>handle</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ds_CMAC_New()
+_____________________________________________________________
+struct </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="9" tint="-0.499984740745262"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>AES_ctx</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> *</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="9" tint="-0.499984740745262"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>ctx</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> = (struct </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="9" tint="-0.499984740745262"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>AES_ctx</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">*)rtlib_calloc(1, sizeof(struct </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="9" tint="-0.499984740745262"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>AES_ctx</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">));
+return </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="9" tint="-0.499984740745262"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
+      </rPr>
+      <t>ctx</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiLight"/>
+        <family val="3"/>
       </rPr>
       <t>;</t>
     </r>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>CSM
+Key</t>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -166,13 +2074,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="15"/>
-      <color theme="1"/>
-      <name val="Bahnschrift"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="9"/>
       <name val="等线"/>
       <family val="3"/>
@@ -183,28 +2084,119 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Cascadia Mono SemiLight"/>
       <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Cascadia Mono SemiLight"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="等线"/>
+      <name val="Cascadia Mono SemiLight"/>
       <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Cascadia Mono SemiLight"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF00FF"/>
+      <name val="Cascadia Mono SemiLight"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Cascadia Mono SemiLight"/>
+      <family val="3"/>
     </font>
     <font>
       <b/>
       <i/>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Cascadia Mono SemiLight"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Cascadia Mono SemiLight"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Cascadia Mono SemiLight"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Cascadia Mono SemiLight"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF92D050"/>
+      <name val="Cascadia Mono SemiLight"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Cascadia Mono SemiLight"/>
       <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Cascadia Mono SemiLight"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Cascadia Mono SemiLight"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="15"/>
+      <color theme="1"/>
+      <name val="Cascadia Mono SemiBold"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Cascadia Mono SemiLight"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="9" tint="-0.499984740745262"/>
+      <name val="Cascadia Mono SemiLight"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="5">
@@ -426,32 +2418,14 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -459,20 +2433,38 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -482,10 +2474,10 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF5050"/>
       <color rgb="FFFF00FF"/>
       <color rgb="FFFDBC53"/>
       <color rgb="FFEB65BE"/>
-      <color rgb="FFFF5050"/>
     </mruColors>
   </colors>
   <extLst>
@@ -798,174 +2790,198 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E38B81CE-79E3-4568-BB50-9E45BADB5D49}">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="22.5" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="133.5" style="1" customWidth="1"/>
+    <col min="1" max="1" width="138.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="147.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="51.375" style="21" customWidth="1"/>
+    <col min="3" max="3" width="51.375" style="31" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="29" t="s">
-        <v>3</v>
+      <c r="A1" s="19" t="s">
+        <v>6</v>
       </c>
       <c r="B1" s="3"/>
-      <c r="C1" s="17"/>
+      <c r="C1" s="27"/>
     </row>
-    <row r="2" spans="1:3" ht="254.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="31" t="s">
+    <row r="2" spans="1:3" ht="275.10000000000002" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="408.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="32" t="s">
-        <v>6</v>
+      <c r="C3" s="25"/>
+    </row>
+    <row r="4" spans="1:3" ht="339.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="18" t="s">
+        <v>11</v>
       </c>
-      <c r="C2" s="18"/>
+      <c r="B4" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="26"/>
     </row>
-    <row r="3" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="6"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="18"/>
+    <row r="5" spans="1:3" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="6"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="19"/>
+    <row r="6" spans="1:3" ht="270" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="25"/>
     </row>
-    <row r="5" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="22"/>
-    </row>
-    <row r="6" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="4"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="23"/>
-    </row>
-    <row r="7" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="4"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="24"/>
+    <row r="7" spans="1:3" ht="114" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="26"/>
     </row>
     <row r="8" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="B8" s="9"/>
-      <c r="C8" s="23"/>
+      <c r="C8" s="24"/>
     </row>
     <row r="9" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6"/>
       <c r="B9" s="8"/>
-      <c r="C9" s="24"/>
+      <c r="C9" s="26"/>
     </row>
     <row r="10" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6"/>
       <c r="B10" s="7"/>
-      <c r="C10" s="25"/>
+      <c r="C10" s="28"/>
     </row>
     <row r="11" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="10"/>
       <c r="B11" s="11"/>
-      <c r="C11" s="23"/>
+      <c r="C11" s="24"/>
     </row>
     <row r="12" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="30" t="s">
-        <v>4</v>
+      <c r="A12" s="17" t="s">
+        <v>3</v>
       </c>
       <c r="B12" s="12"/>
-      <c r="C12" s="17"/>
+      <c r="C12" s="27"/>
     </row>
     <row r="13" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="26" t="s">
+      <c r="A13" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="26"/>
-      <c r="C13" s="26"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
     </row>
     <row r="14" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="15"/>
       <c r="B14" s="16"/>
-      <c r="C14" s="18"/>
+      <c r="C14" s="29"/>
     </row>
     <row r="15" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="6"/>
       <c r="B15" s="7"/>
-      <c r="C15" s="18"/>
+      <c r="C15" s="29"/>
     </row>
     <row r="16" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="6"/>
       <c r="B16" s="8"/>
-      <c r="C16" s="23"/>
+      <c r="C16" s="24"/>
     </row>
     <row r="17" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="6"/>
       <c r="B17" s="7"/>
-      <c r="C17" s="28"/>
+      <c r="C17" s="25"/>
     </row>
     <row r="18" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="6"/>
       <c r="B18" s="8"/>
-      <c r="C18" s="24"/>
+      <c r="C18" s="26"/>
     </row>
     <row r="19" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="6"/>
       <c r="B19" s="9"/>
-      <c r="C19" s="18"/>
+      <c r="C19" s="29"/>
     </row>
     <row r="20" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="27" t="s">
+      <c r="A20" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="27"/>
-      <c r="C20" s="27"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="21"/>
     </row>
     <row r="21" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
       <c r="B21" s="5"/>
-      <c r="C21" s="18"/>
+      <c r="C21" s="29"/>
     </row>
     <row r="22" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="6"/>
       <c r="B22" s="7"/>
-      <c r="C22" s="18"/>
+      <c r="C22" s="29"/>
     </row>
     <row r="23" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="6"/>
       <c r="B23" s="7"/>
-      <c r="C23" s="23"/>
+      <c r="C23" s="24"/>
     </row>
     <row r="24" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="6"/>
       <c r="B24" s="7"/>
-      <c r="C24" s="24"/>
+      <c r="C24" s="26"/>
     </row>
     <row r="25" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="6"/>
       <c r="B25" s="7"/>
-      <c r="C25" s="23"/>
+      <c r="C25" s="24"/>
     </row>
     <row r="26" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="6"/>
       <c r="B26" s="5"/>
-      <c r="C26" s="24"/>
+      <c r="C26" s="26"/>
     </row>
     <row r="27" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="6"/>
       <c r="B27" s="5"/>
-      <c r="C27" s="18"/>
+      <c r="C27" s="29"/>
     </row>
     <row r="28" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="13" t="s">
         <v>2</v>
       </c>
       <c r="B28" s="14"/>
-      <c r="C28" s="20"/>
+      <c r="C28" s="30"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="C6:C7"/>
+  <mergeCells count="9">
+    <mergeCell ref="C2:C4"/>
     <mergeCell ref="C25:C26"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="A13:C13"/>
@@ -973,8 +2989,9 @@
     <mergeCell ref="C16:C18"/>
     <mergeCell ref="C23:C24"/>
     <mergeCell ref="C8:C9"/>
+    <mergeCell ref="C5:C7"/>
   </mergeCells>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
BMW_SecOc add Key-ID Tab
</commit_message>
<xml_diff>
--- a/BMW_SecOc.xlsx
+++ b/BMW_SecOc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DspaceDocument\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git_XuhuaRepo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47E50AE2-281C-4779-A0F4-FB46AA634FEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98C5642B-08C2-43DB-A481-3541F06A36E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="6" xr2:uid="{EE3554E5-5B85-4F6F-95D2-24E55C4E92D2}"/>
+    <workbookView xWindow="28680" yWindow="-8640" windowWidth="38640" windowHeight="21240" activeTab="6" xr2:uid="{EE3554E5-5B85-4F6F-95D2-24E55C4E92D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Code" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,8 @@
     <sheet name="PDU" sheetId="6" r:id="rId4"/>
     <sheet name="PDU_Flow" sheetId="7" r:id="rId5"/>
     <sheet name="Sfn_SecOCMainSetup" sheetId="9" r:id="rId6"/>
-    <sheet name="TxManipulation" sheetId="11" r:id="rId7"/>
+    <sheet name="Key-ID" sheetId="12" r:id="rId7"/>
+    <sheet name="TxManipulation" sheetId="11" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="232">
   <si>
     <t>DsBusCustomCode_onPduFeatureExecutionPrivate(pduFeatureHandle)</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -568,7 +569,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -3264,7 +3265,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -9800,16 +9801,521 @@
 DsBusCustomCodeSecOCRxPduFeature_getEnableVerification</t>
     </r>
   </si>
+  <si>
+    <t>mdlOutputs</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>CollectStaticPduProperties</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>CollectStaticPduPropertiesDuringRuntimeForAllSecOCMsgs</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>CollectStaticPduPropertiesDuringRuntimeForAllSecOCMsgsPerCluster</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">for (unsigned int i = 0; i &lt; filteredSecOCMsgs-&gt;itemCount; i++) {
+    pduFeatData = (UserCode_FeatureData *)GetById(filteredSecOCMsgs, i);
+    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiBold"/>
+        <family val="3"/>
+      </rPr>
+      <t>DsBusCustomCode_collectStaticPduPropertiesDuringRuntime</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono Light"/>
+        <family val="3"/>
+      </rPr>
+      <t>(pduFeatData);
+     if (!pduFeatData-&gt;IsStaticRuntimePropertiesCollected) {
+     ("</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Cascadia Mono Light"/>
+        <family val="3"/>
+      </rPr>
+      <t>Error at message initialization. Some properties could not be identified"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono Light"/>
+        <family val="3"/>
+      </rPr>
+      <t>);
+ }
+ if (pduFeatData-&gt;StaticRuntimeProperiesCollectionRtnVal != E_OK) {
+     ("</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Cascadia Mono Light"/>
+        <family val="3"/>
+      </rPr>
+      <t>Error at message initialization. A getter-function return E_NOT_OK."</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono Light"/>
+        <family val="3"/>
+      </rPr>
+      <t>);
+ }</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>DsBusCustomCode_onPduFeatureExecutionPrivate</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>g_DsBusCustomCode_onPduFeatureExecutionPrivateFunc = DsBusCustomCode_onPduFeatureExecutionPrivate</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">DsBusCustomCode_onPduFeatureExecution(DsBusCustomCodePduFeatureHandle pduFeatureHandle) </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>"internal"</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>dataIdExists</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>!dataIdExists</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>"external"</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>"DataID: %d is not found in dataID_file."</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>"DataID is not defined in cluster database."</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>"Key-id for Message '%s' is missing"</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiBold"/>
+        <family val="3"/>
+      </rPr>
+      <t>DsBusCustomCodeSecuredIPdu_getKeyId(securedIPdu_PduHandle, &amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Cascadia Mono SemiBold"/>
+        <family val="3"/>
+      </rPr>
+      <t>keyId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiBold"/>
+        <family val="3"/>
+      </rPr>
+      <t>);
+DsBusCustomCodeSecuredIPdu_getDataId(securedIPdu_PduHandle, &amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Cascadia Mono SemiBold"/>
+        <family val="3"/>
+      </rPr>
+      <t>dataId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiBold"/>
+        <family val="3"/>
+      </rPr>
+      <t>);</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Cascadia Mono SemiBold"/>
+        <family val="3"/>
+      </rPr>
+      <t>keyId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono Light"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> != 0</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Cascadia Mono SemiBold"/>
+        <family val="3"/>
+      </rPr>
+      <t>keyId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono Light"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> == 0</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFEE0000"/>
+        <rFont val="Cascadia Mono SemiBold"/>
+        <family val="3"/>
+      </rPr>
+      <t>keyId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiBold"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> = GetKeyId(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFEE0000"/>
+        <rFont val="Cascadia Mono SemiBold"/>
+        <family val="3"/>
+      </rPr>
+      <t>dataId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiBold"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFEE0000"/>
+        <rFont val="Cascadia Mono SemiBold"/>
+        <family val="3"/>
+      </rPr>
+      <t>keyId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono Light"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> &gt; 0</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFEE0000"/>
+        <rFont val="Cascadia Mono SemiBold"/>
+        <family val="3"/>
+      </rPr>
+      <t>keyId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono Light"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> == 0</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>if (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFEE0000"/>
+        <rFont val="Cascadia Mono SemiBold"/>
+        <family val="3"/>
+      </rPr>
+      <t>keyId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono Light"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> &lt;= 0)</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">rtnVal = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiBold"/>
+        <family val="3"/>
+      </rPr>
+      <t>DsBusCustomCode_collectStaticPduPropertiesDuringRuntimeEx(pduFeatData)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono Light"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">;
+if (rtnVal != E_OK){
+    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Cascadia Mono Light"/>
+        <family val="3"/>
+      </rPr>
+      <t>"Last error message refers to 'SecuredIPdu_Name'"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono Light"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">
+}</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>if(IsAnyCounterMessage)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>if!(IsAnyCounterMessage)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFEE0000"/>
+        <rFont val="Cascadia Mono SemiBold"/>
+        <family val="3"/>
+      </rPr>
+      <t>keyId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono Light"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> != -1</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>"SecOCSetup"</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>keyId == -1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>"For Rx-Counter-Message '%s' key-id is missing. "
+"For Tx-Counter-Message '%s' key-id is missing. "</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>mdlStart</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>InitDataKeyIdMapping</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>(int)(*inDataKeyIdPairsDataPtr[0])==0</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>(int)(*inDataKeyIdPairsDataPtr[0])!=0</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>if (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="8"/>
+        <rFont val="Cascadia Mono SemiBold"/>
+        <family val="3"/>
+      </rPr>
+      <t>externalKeyIdFileExists</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono Light"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>externalKeyIdFileExists == 0</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>externalKeyIdFileExists == 1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>InitKeyIdsStruct</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SetKeyId(Const_dataId, Const_keyId)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>g_keyids[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFEE0000"/>
+        <rFont val="Cascadia Mono SemiBold"/>
+        <family val="3"/>
+      </rPr>
+      <t>dataId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono Light"/>
+        <family val="3"/>
+      </rPr>
+      <t>].</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFEE0000"/>
+        <rFont val="Cascadia Code SemiBold"/>
+        <family val="3"/>
+      </rPr>
+      <t>keyId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono Light"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> = (uint32)keyId</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="42">
+  <fonts count="50" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -9817,7 +10323,7 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -9826,13 +10332,13 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -9980,7 +10486,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -10096,6 +10602,54 @@
       <name val="Cascadia Code Light"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Cascadia Mono Light"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Cascadia Mono Light"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Cascadia Mono SemiBold"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Cascadia Mono Light"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFEE0000"/>
+      <name val="Cascadia Mono SemiBold"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFEE0000"/>
+      <name val="Cascadia Mono Light"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFEE0000"/>
+      <name val="Cascadia Code SemiBold"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="8"/>
+      <name val="Cascadia Mono SemiBold"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="18">
     <fill>
@@ -10201,7 +10755,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="58">
+  <borders count="67">
     <border>
       <left/>
       <right/>
@@ -10970,11 +11524,144 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="dashed">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="dashed">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="dashed">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="dashed">
+        <color auto="1"/>
+      </right>
+      <top style="dashed">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="dashed">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="dashed">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="dashed">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="dashed">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="dashed">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="dashed">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="202">
+  <cellXfs count="239">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -11328,6 +12015,27 @@
     <xf numFmtId="0" fontId="21" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -11520,26 +12228,110 @@
     <xf numFmtId="0" fontId="5" fillId="15" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="16" borderId="58" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="16" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="16" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="16" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="16" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="16" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="16" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="16" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="16" borderId="62" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="16" borderId="62" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="16" borderId="63" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="16" borderId="64" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="16" borderId="64" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="16" borderId="65" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="16" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="16" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="16" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="16" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="16" borderId="62" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="16" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="16" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="42" fillId="16" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="16" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="16" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="16" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="42" fillId="16" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="16" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -11866,54 +12658,54 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E38B81CE-79E3-4568-BB50-9E45BADB5D49}">
   <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="22"/>
+  <sheetFormatPr defaultRowHeight="22.5" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="138.453125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="154.6328125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="54.90625" style="19" customWidth="1"/>
+    <col min="1" max="1" width="138.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="154.625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="54.875" style="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20.149999999999999" customHeight="1">
+    <row r="1" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="16"/>
     </row>
-    <row r="2" spans="1:3" ht="275.14999999999998" customHeight="1">
+    <row r="2" spans="1:3" ht="275.10000000000002" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>20</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="139" t="s">
+      <c r="C2" s="146" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="409.5" customHeight="1">
+    <row r="3" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>28</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="140"/>
+      <c r="C3" s="147"/>
     </row>
-    <row r="4" spans="1:3" ht="386.25" customHeight="1">
+    <row r="4" spans="1:3" ht="386.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="141"/>
+      <c r="C4" s="148"/>
     </row>
-    <row r="5" spans="1:3" ht="200.25" customHeight="1">
+    <row r="5" spans="1:3" ht="200.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
         <v>31</v>
       </c>
@@ -11924,114 +12716,114 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="22.5" customHeight="1">
+    <row r="6" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5"/>
       <c r="B6" s="6"/>
       <c r="C6" s="17"/>
     </row>
-    <row r="7" spans="1:3" ht="20.149999999999999" customHeight="1">
+    <row r="7" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="16"/>
     </row>
-    <row r="8" spans="1:3" ht="20.149999999999999" customHeight="1">
+    <row r="8" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>77</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="16"/>
     </row>
-    <row r="9" spans="1:3" ht="74.25" customHeight="1">
-      <c r="A9" s="147" t="s">
+    <row r="9" spans="1:3" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="154" t="s">
         <v>140</v>
       </c>
-      <c r="B9" s="147"/>
-      <c r="C9" s="148"/>
+      <c r="B9" s="154"/>
+      <c r="C9" s="155"/>
     </row>
-    <row r="10" spans="1:3" ht="287.25" customHeight="1">
+    <row r="10" spans="1:3" ht="287.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="95" t="s">
         <v>174</v>
       </c>
       <c r="B10" s="96" t="s">
         <v>74</v>
       </c>
-      <c r="C10" s="142" t="s">
+      <c r="C10" s="149" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="159.75" customHeight="1">
+    <row r="11" spans="1:3" ht="159.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="95" t="s">
         <v>78</v>
       </c>
       <c r="B11" s="96" t="s">
         <v>141</v>
       </c>
-      <c r="C11" s="143"/>
+      <c r="C11" s="150"/>
     </row>
-    <row r="12" spans="1:3" ht="257.25" customHeight="1">
-      <c r="A12" s="145" t="s">
+    <row r="12" spans="1:3" ht="257.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="152" t="s">
         <v>142</v>
       </c>
       <c r="B12" s="96" t="s">
         <v>80</v>
       </c>
-      <c r="C12" s="143"/>
+      <c r="C12" s="150"/>
     </row>
-    <row r="13" spans="1:3" ht="120.75" customHeight="1">
-      <c r="A13" s="146"/>
+    <row r="13" spans="1:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="153"/>
       <c r="B13" s="96" t="s">
         <v>79</v>
       </c>
-      <c r="C13" s="144"/>
+      <c r="C13" s="151"/>
     </row>
-    <row r="14" spans="1:3" ht="157.5" customHeight="1">
+    <row r="14" spans="1:3" ht="157.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="98" t="s">
         <v>143</v>
       </c>
       <c r="B14" s="96" t="s">
         <v>144</v>
       </c>
-      <c r="C14" s="142" t="s">
+      <c r="C14" s="149" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="123.75" customHeight="1">
+    <row r="15" spans="1:3" ht="123.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="96" t="s">
         <v>145</v>
       </c>
       <c r="B15" s="96" t="s">
         <v>146</v>
       </c>
-      <c r="C15" s="144"/>
+      <c r="C15" s="151"/>
     </row>
-    <row r="16" spans="1:3" ht="378.75" customHeight="1">
+    <row r="16" spans="1:3" ht="378.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
         <v>37</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="C16" s="139"/>
+      <c r="C16" s="146"/>
     </row>
-    <row r="17" spans="1:3" ht="110.15" customHeight="1">
+    <row r="17" spans="1:3" ht="110.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="140"/>
+      <c r="C17" s="147"/>
     </row>
-    <row r="18" spans="1:3" ht="20.149999999999999" customHeight="1">
+    <row r="18" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="43" t="s">
         <v>5</v>
       </c>
       <c r="B18" s="44"/>
       <c r="C18" s="45"/>
     </row>
-    <row r="19" spans="1:3" ht="390.75" customHeight="1">
+    <row r="19" spans="1:3" ht="390.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
         <v>61</v>
       </c>
@@ -12042,166 +12834,166 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="223.5" customHeight="1">
+    <row r="20" spans="1:3" ht="223.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
         <v>48</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="C20" s="136" t="s">
+      <c r="C20" s="143" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="40" customHeight="1">
-      <c r="A21" s="195" t="s">
+    <row r="21" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="131" t="s">
         <v>172</v>
       </c>
-      <c r="B21" s="196"/>
-      <c r="C21" s="137"/>
+      <c r="B21" s="132"/>
+      <c r="C21" s="144"/>
     </row>
-    <row r="22" spans="1:3" ht="42.75" customHeight="1">
+    <row r="22" spans="1:3" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
         <v>16</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C22" s="137"/>
+      <c r="C22" s="144"/>
     </row>
-    <row r="23" spans="1:3" ht="370.5" customHeight="1">
+    <row r="23" spans="1:3" ht="370.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
         <v>15</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C23" s="138"/>
+      <c r="C23" s="145"/>
     </row>
-    <row r="24" spans="1:3" ht="78.75" customHeight="1">
+    <row r="24" spans="1:3" ht="78.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
         <v>10</v>
       </c>
       <c r="B24" s="4"/>
-      <c r="C24" s="135" t="s">
+      <c r="C24" s="142" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="36.65" customHeight="1">
+    <row r="25" spans="1:3" ht="36.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="s">
         <v>11</v>
       </c>
       <c r="B25" s="4"/>
-      <c r="C25" s="135"/>
+      <c r="C25" s="142"/>
     </row>
-    <row r="26" spans="1:3" ht="67.5" customHeight="1">
+    <row r="26" spans="1:3" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
         <v>12</v>
       </c>
       <c r="B26" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="135"/>
+      <c r="C26" s="142"/>
     </row>
-    <row r="27" spans="1:3" ht="242.25" customHeight="1">
+    <row r="27" spans="1:3" ht="242.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="10" t="s">
         <v>119</v>
       </c>
       <c r="B27" s="10" t="s">
         <v>184</v>
       </c>
-      <c r="C27" s="135"/>
+      <c r="C27" s="142"/>
     </row>
-    <row r="28" spans="1:3" ht="110.15" customHeight="1">
+    <row r="28" spans="1:3" ht="110.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
         <v>13</v>
       </c>
       <c r="B28" s="12"/>
-      <c r="C28" s="135"/>
+      <c r="C28" s="142"/>
     </row>
-    <row r="29" spans="1:3" ht="224.5" customHeight="1">
+    <row r="29" spans="1:3" ht="224.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="12" t="s">
         <v>60</v>
       </c>
       <c r="B29" s="12"/>
-      <c r="C29" s="135"/>
+      <c r="C29" s="142"/>
     </row>
-    <row r="30" spans="1:3" ht="40" customHeight="1">
-      <c r="A30" s="197" t="s">
+    <row r="30" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="133" t="s">
         <v>173</v>
       </c>
-      <c r="B30" s="197"/>
-      <c r="C30" s="135"/>
+      <c r="B30" s="133"/>
+      <c r="C30" s="142"/>
     </row>
-    <row r="31" spans="1:3" ht="70.5" customHeight="1">
+    <row r="31" spans="1:3" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="12" t="s">
         <v>98</v>
       </c>
       <c r="B31" s="12"/>
-      <c r="C31" s="132"/>
+      <c r="C31" s="139"/>
     </row>
-    <row r="32" spans="1:3" ht="20.149999999999999" customHeight="1">
+    <row r="32" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="43" t="s">
         <v>57</v>
       </c>
       <c r="B32" s="46"/>
       <c r="C32" s="47"/>
     </row>
-    <row r="33" spans="1:3" ht="174" customHeight="1">
+    <row r="33" spans="1:3" ht="174" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="12" t="s">
         <v>62</v>
       </c>
       <c r="B33" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="C33" s="131" t="s">
+      <c r="C33" s="138" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="102" customHeight="1">
+    <row r="34" spans="1:3" ht="102" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="12" t="s">
         <v>64</v>
       </c>
       <c r="B34" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="C34" s="132"/>
+      <c r="C34" s="139"/>
     </row>
-    <row r="35" spans="1:3" ht="234.65" customHeight="1">
-      <c r="A35" s="133" t="s">
+    <row r="35" spans="1:3" ht="234.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="140" t="s">
         <v>65</v>
       </c>
       <c r="B35" s="49" t="s">
         <v>169</v>
       </c>
-      <c r="C35" s="131" t="s">
+      <c r="C35" s="138" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="215.15" customHeight="1">
-      <c r="A36" s="134"/>
+    <row r="36" spans="1:3" ht="215.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="141"/>
       <c r="B36" s="12" t="s">
         <v>171</v>
       </c>
-      <c r="C36" s="135"/>
+      <c r="C36" s="142"/>
     </row>
-    <row r="37" spans="1:3" ht="297.75" customHeight="1">
-      <c r="A37" s="134"/>
+    <row r="37" spans="1:3" ht="297.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="141"/>
       <c r="B37" s="12" t="s">
         <v>170</v>
       </c>
-      <c r="C37" s="135"/>
+      <c r="C37" s="142"/>
     </row>
-    <row r="38" spans="1:3" ht="135.5" customHeight="1">
+    <row r="38" spans="1:3" ht="135.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="12" t="s">
         <v>70</v>
       </c>
       <c r="B38" s="12" t="s">
         <v>190</v>
       </c>
-      <c r="C38" s="132"/>
+      <c r="C38" s="139"/>
     </row>
-    <row r="39" spans="1:3" ht="393.75" customHeight="1">
+    <row r="39" spans="1:3" ht="393.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="12" t="s">
         <v>191</v>
       </c>
@@ -12212,7 +13004,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="40" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="11">
     <mergeCell ref="C33:C34"/>
@@ -12241,98 +13033,98 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="49.26953125" style="50" customWidth="1"/>
-    <col min="3" max="3" width="65.453125" customWidth="1"/>
+    <col min="2" max="2" width="49.25" style="50" customWidth="1"/>
+    <col min="3" max="3" width="65.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" ht="20.149999999999999" customHeight="1">
-      <c r="B3" s="149" t="s">
+    <row r="3" spans="2:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="156" t="s">
         <v>109</v>
       </c>
       <c r="C3" s="90" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="20.149999999999999" customHeight="1">
-      <c r="B4" s="151"/>
+    <row r="4" spans="2:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="158"/>
       <c r="C4" s="90" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="20.149999999999999" customHeight="1">
+    <row r="5" spans="2:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="78" t="s">
         <v>111</v>
       </c>
       <c r="C5" s="91"/>
     </row>
-    <row r="6" spans="2:3" ht="20.149999999999999" customHeight="1">
-      <c r="B6" s="149" t="s">
+    <row r="6" spans="2:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="156" t="s">
         <v>110</v>
       </c>
       <c r="C6" s="90" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="7" spans="2:3" ht="20.149999999999999" customHeight="1">
-      <c r="B7" s="150"/>
+    <row r="7" spans="2:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="157"/>
       <c r="C7" s="90" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="8" spans="2:3" ht="20.149999999999999" customHeight="1">
-      <c r="B8" s="150"/>
+    <row r="8" spans="2:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="157"/>
       <c r="C8" s="90" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="9" spans="2:3" ht="20.149999999999999" customHeight="1">
-      <c r="B9" s="151"/>
+    <row r="9" spans="2:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="158"/>
       <c r="C9" s="90" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="10" spans="2:3" ht="20.149999999999999" customHeight="1">
+    <row r="10" spans="2:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="89" t="s">
         <v>118</v>
       </c>
       <c r="C10" s="91"/>
     </row>
-    <row r="11" spans="2:3" ht="20.149999999999999" customHeight="1">
+    <row r="11" spans="2:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="89" t="s">
         <v>73</v>
       </c>
       <c r="C11" s="91"/>
     </row>
-    <row r="12" spans="2:3" ht="65.25" customHeight="1">
-      <c r="B12" s="152" t="s">
+    <row r="12" spans="2:3" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="159" t="s">
         <v>71</v>
       </c>
       <c r="C12" s="92" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="13" spans="2:3" ht="80.25" customHeight="1">
-      <c r="B13" s="153"/>
+    <row r="13" spans="2:3" ht="80.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="160"/>
       <c r="C13" s="92" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="14" spans="2:3" ht="20.149999999999999" customHeight="1">
+    <row r="14" spans="2:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="22"/>
     </row>
-    <row r="15" spans="2:3" ht="20.149999999999999" customHeight="1">
+    <row r="15" spans="2:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="79" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="16" spans="2:3" ht="20.149999999999999" customHeight="1">
+    <row r="16" spans="2:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="79" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="2:2" ht="20.149999999999999" customHeight="1">
+    <row r="17" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="79" t="s">
         <v>71</v>
       </c>
@@ -12356,42 +13148,42 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.36328125" style="20" customWidth="1"/>
-    <col min="2" max="2" width="21.26953125" style="14" customWidth="1"/>
-    <col min="3" max="3" width="28.453125" style="14" customWidth="1"/>
-    <col min="4" max="4" width="26.08984375" style="21" customWidth="1"/>
+    <col min="1" max="1" width="28.375" style="20" customWidth="1"/>
+    <col min="2" max="2" width="21.25" style="14" customWidth="1"/>
+    <col min="3" max="3" width="28.5" style="14" customWidth="1"/>
+    <col min="4" max="4" width="26.125" style="21" customWidth="1"/>
     <col min="5" max="5" width="63" style="14" customWidth="1"/>
-    <col min="6" max="6" width="37.6328125" style="14" customWidth="1"/>
-    <col min="7" max="7" width="70.6328125" style="13" customWidth="1"/>
-    <col min="8" max="8" width="57.90625" style="13" customWidth="1"/>
-    <col min="9" max="9" width="82.453125" style="13" customWidth="1"/>
-    <col min="10" max="10" width="89.6328125" style="13" customWidth="1"/>
-    <col min="11" max="11" width="46.08984375" style="13" customWidth="1"/>
-    <col min="12" max="12" width="51.453125" style="13" customWidth="1"/>
+    <col min="6" max="6" width="37.625" style="14" customWidth="1"/>
+    <col min="7" max="7" width="70.625" style="13" customWidth="1"/>
+    <col min="8" max="8" width="57.875" style="13" customWidth="1"/>
+    <col min="9" max="9" width="82.5" style="13" customWidth="1"/>
+    <col min="10" max="10" width="89.625" style="13" customWidth="1"/>
+    <col min="11" max="11" width="46.125" style="13" customWidth="1"/>
+    <col min="12" max="12" width="51.5" style="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="203.5" customHeight="1">
-      <c r="A1" s="154" t="s">
+    <row r="1" spans="1:12" ht="203.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="161" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="161" t="s">
+      <c r="B1" s="168" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="160" t="s">
+      <c r="C1" s="167" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="160" t="s">
+      <c r="D1" s="167" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="160" t="s">
+      <c r="E1" s="167" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="160" t="s">
+      <c r="F1" s="167" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="160" t="s">
+      <c r="G1" s="167" t="s">
         <v>45</v>
       </c>
       <c r="H1" s="108" t="s">
@@ -12404,14 +13196,14 @@
       <c r="K1" s="107"/>
       <c r="L1" s="109"/>
     </row>
-    <row r="2" spans="1:12" ht="287.5" customHeight="1">
-      <c r="A2" s="155"/>
-      <c r="B2" s="157"/>
-      <c r="C2" s="159"/>
-      <c r="D2" s="159"/>
-      <c r="E2" s="159"/>
-      <c r="F2" s="159"/>
-      <c r="G2" s="159"/>
+    <row r="2" spans="1:12" ht="287.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="162"/>
+      <c r="B2" s="164"/>
+      <c r="C2" s="166"/>
+      <c r="D2" s="166"/>
+      <c r="E2" s="166"/>
+      <c r="F2" s="166"/>
+      <c r="G2" s="166"/>
       <c r="H2" s="110" t="s">
         <v>41</v>
       </c>
@@ -12426,15 +13218,15 @@
       </c>
       <c r="L2" s="112"/>
     </row>
-    <row r="3" spans="1:12" ht="53.25" customHeight="1">
-      <c r="A3" s="155"/>
-      <c r="B3" s="157"/>
-      <c r="C3" s="159"/>
-      <c r="D3" s="159"/>
-      <c r="E3" s="159" t="s">
+    <row r="3" spans="1:12" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="162"/>
+      <c r="B3" s="164"/>
+      <c r="C3" s="166"/>
+      <c r="D3" s="166"/>
+      <c r="E3" s="166" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="162" t="s">
+      <c r="F3" s="169" t="s">
         <v>33</v>
       </c>
       <c r="G3" s="110" t="s">
@@ -12446,17 +13238,17 @@
       <c r="K3" s="110"/>
       <c r="L3" s="112"/>
     </row>
-    <row r="4" spans="1:12" ht="233.15" customHeight="1">
-      <c r="A4" s="155"/>
-      <c r="B4" s="157"/>
-      <c r="C4" s="159"/>
-      <c r="D4" s="159"/>
-      <c r="E4" s="159"/>
-      <c r="F4" s="162"/>
-      <c r="G4" s="159" t="s">
+    <row r="4" spans="1:12" ht="233.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="162"/>
+      <c r="B4" s="164"/>
+      <c r="C4" s="166"/>
+      <c r="D4" s="166"/>
+      <c r="E4" s="166"/>
+      <c r="F4" s="169"/>
+      <c r="G4" s="166" t="s">
         <v>35</v>
       </c>
-      <c r="H4" s="159" t="s">
+      <c r="H4" s="166" t="s">
         <v>81</v>
       </c>
       <c r="I4" s="111" t="s">
@@ -12468,15 +13260,15 @@
       <c r="K4" s="110"/>
       <c r="L4" s="112"/>
     </row>
-    <row r="5" spans="1:12" ht="113.15" customHeight="1">
-      <c r="A5" s="155"/>
-      <c r="B5" s="157"/>
-      <c r="C5" s="159"/>
-      <c r="D5" s="159"/>
-      <c r="E5" s="159"/>
-      <c r="F5" s="162"/>
-      <c r="G5" s="159"/>
-      <c r="H5" s="159"/>
+    <row r="5" spans="1:12" ht="113.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="162"/>
+      <c r="B5" s="164"/>
+      <c r="C5" s="166"/>
+      <c r="D5" s="166"/>
+      <c r="E5" s="166"/>
+      <c r="F5" s="169"/>
+      <c r="G5" s="166"/>
+      <c r="H5" s="166"/>
       <c r="I5" s="111" t="s">
         <v>82</v>
       </c>
@@ -12490,11 +13282,11 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="160.5" customHeight="1">
-      <c r="A6" s="155"/>
-      <c r="B6" s="157"/>
-      <c r="C6" s="159"/>
-      <c r="D6" s="159"/>
+    <row r="6" spans="1:12" ht="160.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="162"/>
+      <c r="B6" s="164"/>
+      <c r="C6" s="166"/>
+      <c r="D6" s="166"/>
       <c r="E6" s="110" t="s">
         <v>32</v>
       </c>
@@ -12506,9 +13298,9 @@
       <c r="K6" s="110"/>
       <c r="L6" s="112"/>
     </row>
-    <row r="7" spans="1:12" ht="30" customHeight="1">
-      <c r="A7" s="155"/>
-      <c r="B7" s="157" t="s">
+    <row r="7" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="162"/>
+      <c r="B7" s="164" t="s">
         <v>38</v>
       </c>
       <c r="C7" s="113" t="s">
@@ -12524,9 +13316,9 @@
       <c r="K7" s="110"/>
       <c r="L7" s="112"/>
     </row>
-    <row r="8" spans="1:12" ht="30" customHeight="1">
-      <c r="A8" s="155"/>
-      <c r="B8" s="157"/>
+    <row r="8" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="162"/>
+      <c r="B8" s="164"/>
       <c r="C8" s="113" t="s">
         <v>40</v>
       </c>
@@ -12540,9 +13332,9 @@
       <c r="K8" s="110"/>
       <c r="L8" s="112"/>
     </row>
-    <row r="9" spans="1:12" ht="30" customHeight="1">
-      <c r="A9" s="155"/>
-      <c r="B9" s="157"/>
+    <row r="9" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="162"/>
+      <c r="B9" s="164"/>
       <c r="C9" s="113" t="s">
         <v>75</v>
       </c>
@@ -12556,9 +13348,9 @@
       <c r="K9" s="110"/>
       <c r="L9" s="112"/>
     </row>
-    <row r="10" spans="1:12" ht="30" customHeight="1">
-      <c r="A10" s="155"/>
-      <c r="B10" s="157"/>
+    <row r="10" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="162"/>
+      <c r="B10" s="164"/>
       <c r="C10" s="113" t="s">
         <v>76</v>
       </c>
@@ -12572,9 +13364,9 @@
       <c r="K10" s="110"/>
       <c r="L10" s="112"/>
     </row>
-    <row r="11" spans="1:12" ht="30" customHeight="1">
-      <c r="A11" s="155"/>
-      <c r="B11" s="163" t="s">
+    <row r="11" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="162"/>
+      <c r="B11" s="170" t="s">
         <v>67</v>
       </c>
       <c r="C11" s="14" t="s">
@@ -12590,9 +13382,9 @@
       <c r="K11" s="110"/>
       <c r="L11" s="112"/>
     </row>
-    <row r="12" spans="1:12" ht="30" customHeight="1">
-      <c r="A12" s="155"/>
-      <c r="B12" s="164"/>
+    <row r="12" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="162"/>
+      <c r="B12" s="171"/>
       <c r="C12" s="113" t="s">
         <v>166</v>
       </c>
@@ -12606,9 +13398,9 @@
       <c r="K12" s="110"/>
       <c r="L12" s="112"/>
     </row>
-    <row r="13" spans="1:12" ht="30" customHeight="1">
-      <c r="A13" s="155"/>
-      <c r="B13" s="165"/>
+    <row r="13" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="162"/>
+      <c r="B13" s="172"/>
       <c r="C13" s="113" t="s">
         <v>167</v>
       </c>
@@ -12622,9 +13414,9 @@
       <c r="K13" s="110"/>
       <c r="L13" s="112"/>
     </row>
-    <row r="14" spans="1:12" ht="30" customHeight="1">
-      <c r="A14" s="155"/>
-      <c r="B14" s="163" t="s">
+    <row r="14" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="162"/>
+      <c r="B14" s="170" t="s">
         <v>69</v>
       </c>
       <c r="C14" s="113" t="s">
@@ -12640,9 +13432,9 @@
       <c r="K14" s="110"/>
       <c r="L14" s="112"/>
     </row>
-    <row r="15" spans="1:12" ht="30" customHeight="1">
-      <c r="A15" s="155"/>
-      <c r="B15" s="164"/>
+    <row r="15" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="162"/>
+      <c r="B15" s="171"/>
       <c r="C15" s="113" t="s">
         <v>179</v>
       </c>
@@ -12656,9 +13448,9 @@
       <c r="K15" s="110"/>
       <c r="L15" s="112"/>
     </row>
-    <row r="16" spans="1:12" ht="30" customHeight="1">
-      <c r="A16" s="155"/>
-      <c r="B16" s="165"/>
+    <row r="16" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="162"/>
+      <c r="B16" s="172"/>
       <c r="C16" s="113" t="s">
         <v>68</v>
       </c>
@@ -12672,9 +13464,9 @@
       <c r="K16" s="110"/>
       <c r="L16" s="112"/>
     </row>
-    <row r="17" spans="1:12" ht="30" customHeight="1">
-      <c r="A17" s="155"/>
-      <c r="B17" s="157" t="s">
+    <row r="17" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="162"/>
+      <c r="B17" s="164" t="s">
         <v>159</v>
       </c>
       <c r="C17" s="113" t="s">
@@ -12690,9 +13482,9 @@
       <c r="K17" s="110"/>
       <c r="L17" s="112"/>
     </row>
-    <row r="18" spans="1:12" ht="30" customHeight="1">
-      <c r="A18" s="156"/>
-      <c r="B18" s="158"/>
+    <row r="18" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="163"/>
+      <c r="B18" s="165"/>
       <c r="C18" s="115" t="s">
         <v>161</v>
       </c>
@@ -12737,19 +13529,19 @@
       <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.08984375" style="23" customWidth="1"/>
-    <col min="2" max="2" width="20.7265625" customWidth="1"/>
-    <col min="3" max="6" width="20.6328125" style="23" customWidth="1"/>
+    <col min="1" max="1" width="20.125" style="23" customWidth="1"/>
+    <col min="2" max="2" width="20.75" customWidth="1"/>
+    <col min="3" max="6" width="20.625" style="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1"/>
-    <row r="2" spans="1:6" ht="30" customHeight="1">
-      <c r="A2" s="166" t="s">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="173" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="168" t="s">
+      <c r="B2" s="175" t="s">
         <v>50</v>
       </c>
       <c r="C2" s="24" t="s">
@@ -12765,17 +13557,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="30" customHeight="1">
-      <c r="A3" s="167"/>
-      <c r="B3" s="169"/>
+    <row r="3" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="174"/>
+      <c r="B3" s="176"/>
       <c r="C3" s="40"/>
       <c r="D3" s="41"/>
       <c r="E3" s="41"/>
       <c r="F3" s="42"/>
     </row>
-    <row r="4" spans="1:6" ht="30" customHeight="1">
-      <c r="A4" s="167"/>
-      <c r="B4" s="169" t="s">
+    <row r="4" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="174"/>
+      <c r="B4" s="176" t="s">
         <v>51</v>
       </c>
       <c r="C4" s="30" t="s">
@@ -12791,9 +13583,9 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="30" customHeight="1">
-      <c r="A5" s="167"/>
-      <c r="B5" s="169"/>
+    <row r="5" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="174"/>
+      <c r="B5" s="176"/>
       <c r="C5" s="34" t="s">
         <v>54</v>
       </c>
@@ -12801,11 +13593,11 @@
       <c r="E5" s="28"/>
       <c r="F5" s="29"/>
     </row>
-    <row r="6" spans="1:6" ht="30" customHeight="1">
-      <c r="A6" s="167" t="s">
+    <row r="6" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="174" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="169" t="s">
+      <c r="B6" s="176" t="s">
         <v>50</v>
       </c>
       <c r="C6" s="30" t="s">
@@ -12819,17 +13611,17 @@
       </c>
       <c r="F6" s="29"/>
     </row>
-    <row r="7" spans="1:6" ht="30" customHeight="1">
-      <c r="A7" s="167"/>
-      <c r="B7" s="169"/>
+    <row r="7" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="174"/>
+      <c r="B7" s="176"/>
       <c r="C7" s="40"/>
       <c r="D7" s="41"/>
       <c r="E7" s="41"/>
       <c r="F7" s="42"/>
     </row>
-    <row r="8" spans="1:6" ht="30" customHeight="1">
-      <c r="A8" s="167"/>
-      <c r="B8" s="169" t="s">
+    <row r="8" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="174"/>
+      <c r="B8" s="176" t="s">
         <v>51</v>
       </c>
       <c r="C8" s="30" t="s">
@@ -12843,9 +13635,9 @@
       </c>
       <c r="F8" s="29"/>
     </row>
-    <row r="9" spans="1:6" ht="30" customHeight="1" thickBot="1">
-      <c r="A9" s="170"/>
-      <c r="B9" s="171"/>
+    <row r="9" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="177"/>
+      <c r="B9" s="178"/>
       <c r="C9" s="37" t="s">
         <v>54</v>
       </c>
@@ -12875,27 +13667,27 @@
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.7265625" customWidth="1"/>
-    <col min="2" max="2" width="38.7265625" customWidth="1"/>
-    <col min="3" max="3" width="59.90625" customWidth="1"/>
-    <col min="4" max="4" width="48.7265625" customWidth="1"/>
-    <col min="5" max="5" width="36.7265625" customWidth="1"/>
-    <col min="6" max="6" width="62.36328125" customWidth="1"/>
+    <col min="1" max="1" width="3.75" customWidth="1"/>
+    <col min="2" max="2" width="38.75" customWidth="1"/>
+    <col min="3" max="3" width="59.875" customWidth="1"/>
+    <col min="4" max="4" width="48.75" customWidth="1"/>
+    <col min="5" max="5" width="36.75" customWidth="1"/>
+    <col min="6" max="6" width="62.375" customWidth="1"/>
     <col min="7" max="7" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" ht="16">
-      <c r="B2" s="174" t="s">
+    <row r="2" spans="2:6" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="B2" s="181" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="175"/>
-      <c r="D2" s="175"/>
-      <c r="E2" s="175"/>
-      <c r="F2" s="176"/>
+      <c r="C2" s="182"/>
+      <c r="D2" s="182"/>
+      <c r="E2" s="182"/>
+      <c r="F2" s="183"/>
     </row>
-    <row r="3" spans="2:6" ht="16.5" thickBot="1">
+    <row r="3" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="53" t="s">
         <v>88</v>
       </c>
@@ -12908,7 +13700,7 @@
       </c>
       <c r="F3" s="57"/>
     </row>
-    <row r="4" spans="2:6" ht="16">
+    <row r="4" spans="2:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B4" s="52"/>
       <c r="C4" s="69" t="s">
         <v>92</v>
@@ -12917,7 +13709,7 @@
       <c r="E4" s="51"/>
       <c r="F4" s="57"/>
     </row>
-    <row r="5" spans="2:6" ht="16">
+    <row r="5" spans="2:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B5" s="52"/>
       <c r="C5" s="54" t="s">
         <v>102</v>
@@ -12926,7 +13718,7 @@
       <c r="E5" s="51"/>
       <c r="F5" s="57"/>
     </row>
-    <row r="6" spans="2:6" ht="16">
+    <row r="6" spans="2:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B6" s="52"/>
       <c r="C6" s="54" t="s">
         <v>90</v>
@@ -12937,7 +13729,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="16.5" thickBot="1">
+    <row r="7" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="70"/>
       <c r="C7" s="54" t="s">
         <v>89</v>
@@ -12948,7 +13740,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="24.75" customHeight="1">
+    <row r="8" spans="2:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="71" t="s">
         <v>58</v>
       </c>
@@ -12965,7 +13757,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="16">
+    <row r="9" spans="2:6" ht="16.5" x14ac:dyDescent="0.2">
       <c r="B9" s="88"/>
       <c r="C9" s="83"/>
       <c r="D9" s="65" t="s">
@@ -12974,16 +13766,16 @@
       <c r="E9" s="82"/>
       <c r="F9" s="73"/>
     </row>
-    <row r="10" spans="2:6" ht="16">
-      <c r="B10" s="172" t="s">
+    <row r="10" spans="2:6" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="B10" s="179" t="s">
         <v>94</v>
       </c>
-      <c r="C10" s="173"/>
+      <c r="C10" s="180"/>
       <c r="D10" s="65"/>
       <c r="E10" s="83"/>
       <c r="F10" s="73"/>
     </row>
-    <row r="11" spans="2:6" ht="16.5" thickBot="1">
+    <row r="11" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B11" s="87"/>
       <c r="C11" s="72" t="s">
         <v>117</v>
@@ -12992,7 +13784,7 @@
       <c r="E11" s="84"/>
       <c r="F11" s="73"/>
     </row>
-    <row r="12" spans="2:6" ht="16.5" thickBot="1">
+    <row r="12" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="86"/>
       <c r="C12" s="85"/>
       <c r="D12" s="81" t="s">
@@ -13001,7 +13793,7 @@
       <c r="E12" s="84"/>
       <c r="F12" s="73"/>
     </row>
-    <row r="13" spans="2:6" ht="16.5" thickBot="1">
+    <row r="13" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B13" s="77"/>
       <c r="C13" s="57"/>
       <c r="D13" s="76"/>
@@ -13010,14 +13802,14 @@
       </c>
       <c r="F13" s="73"/>
     </row>
-    <row r="14" spans="2:6">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B14" s="77"/>
       <c r="C14" s="57"/>
       <c r="D14" s="57"/>
       <c r="E14" s="76"/>
       <c r="F14" s="59"/>
     </row>
-    <row r="15" spans="2:6" ht="16.5" thickBot="1">
+    <row r="15" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B15" s="77"/>
       <c r="C15" s="61" t="s">
         <v>95</v>
@@ -13028,7 +13820,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="2:6" ht="16">
+    <row r="16" spans="2:6" ht="16.5" x14ac:dyDescent="0.2">
       <c r="B16" s="77"/>
       <c r="C16" s="61" t="s">
         <v>96</v>
@@ -13037,7 +13829,7 @@
       <c r="E16" s="58"/>
       <c r="F16" s="74"/>
     </row>
-    <row r="17" spans="2:6" ht="16">
+    <row r="17" spans="2:6" ht="16.5" x14ac:dyDescent="0.2">
       <c r="B17" s="77"/>
       <c r="C17" s="64" t="s">
         <v>116</v>
@@ -13048,7 +13840,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="16">
+    <row r="18" spans="2:6" ht="16.5" x14ac:dyDescent="0.2">
       <c r="B18" s="77"/>
       <c r="C18" s="57"/>
       <c r="D18" s="64" t="s">
@@ -13057,7 +13849,7 @@
       <c r="E18" s="58"/>
       <c r="F18" s="57"/>
     </row>
-    <row r="19" spans="2:6" ht="16">
+    <row r="19" spans="2:6" ht="16.5" x14ac:dyDescent="0.2">
       <c r="B19" s="77"/>
       <c r="C19" s="57"/>
       <c r="D19" s="57"/>
@@ -13081,26 +13873,26 @@
   <dimension ref="B1:G17"/>
   <sheetViews>
     <sheetView topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:E5"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.6328125" customWidth="1"/>
-    <col min="2" max="2" width="36.453125" style="93" customWidth="1"/>
-    <col min="3" max="3" width="35.453125" style="93" customWidth="1"/>
-    <col min="4" max="4" width="89.08984375" style="93" customWidth="1"/>
-    <col min="5" max="5" width="85.90625" style="94" customWidth="1"/>
-    <col min="6" max="6" width="86.36328125" style="94" customWidth="1"/>
-    <col min="7" max="7" width="85.90625" style="97" customWidth="1"/>
+    <col min="1" max="1" width="2.625" customWidth="1"/>
+    <col min="2" max="2" width="36.5" style="93" customWidth="1"/>
+    <col min="3" max="3" width="35.5" style="93" customWidth="1"/>
+    <col min="4" max="4" width="89.125" style="93" customWidth="1"/>
+    <col min="5" max="5" width="85.875" style="94" customWidth="1"/>
+    <col min="6" max="6" width="86.375" style="94" customWidth="1"/>
+    <col min="7" max="7" width="85.875" style="97" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="15" customHeight="1"/>
-    <row r="2" spans="2:7" ht="150.75" customHeight="1">
-      <c r="B2" s="177" t="s">
+    <row r="1" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:7" ht="150.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="184" t="s">
         <v>150</v>
       </c>
-      <c r="C2" s="179" t="s">
+      <c r="C2" s="186" t="s">
         <v>151</v>
       </c>
       <c r="D2" s="119" t="s">
@@ -13112,9 +13904,9 @@
       <c r="F2" s="121"/>
       <c r="G2" s="122"/>
     </row>
-    <row r="3" spans="2:7" ht="176.25" customHeight="1">
-      <c r="B3" s="178"/>
-      <c r="C3" s="180"/>
+    <row r="3" spans="2:7" ht="176.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="185"/>
+      <c r="C3" s="187"/>
       <c r="D3" s="123" t="s">
         <v>153</v>
       </c>
@@ -13124,15 +13916,15 @@
       <c r="F3" s="124"/>
       <c r="G3" s="125"/>
     </row>
-    <row r="4" spans="2:7" ht="191.25" customHeight="1">
-      <c r="B4" s="192" t="s">
+    <row r="4" spans="2:7" ht="191.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="199" t="s">
         <v>123</v>
       </c>
-      <c r="C4" s="181" t="s">
+      <c r="C4" s="188" t="s">
         <v>127</v>
       </c>
-      <c r="D4" s="181"/>
-      <c r="E4" s="190" t="s">
+      <c r="D4" s="188"/>
+      <c r="E4" s="197" t="s">
         <v>139</v>
       </c>
       <c r="F4" s="99" t="s">
@@ -13142,11 +13934,11 @@
         <v>130</v>
       </c>
     </row>
-    <row r="5" spans="2:7" ht="100" customHeight="1">
-      <c r="B5" s="193"/>
-      <c r="C5" s="182"/>
-      <c r="D5" s="182"/>
-      <c r="E5" s="191"/>
+    <row r="5" spans="2:7" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="200"/>
+      <c r="C5" s="189"/>
+      <c r="D5" s="189"/>
+      <c r="E5" s="198"/>
       <c r="F5" s="102" t="s">
         <v>129</v>
       </c>
@@ -13154,9 +13946,9 @@
         <v>131</v>
       </c>
     </row>
-    <row r="6" spans="2:7" ht="79.5" customHeight="1">
-      <c r="B6" s="193"/>
-      <c r="C6" s="182" t="s">
+    <row r="6" spans="2:7" ht="79.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="200"/>
+      <c r="C6" s="189" t="s">
         <v>124</v>
       </c>
       <c r="D6" s="102" t="s">
@@ -13168,9 +13960,9 @@
       <c r="F6" s="127"/>
       <c r="G6" s="128"/>
     </row>
-    <row r="7" spans="2:7" ht="155.25" customHeight="1">
-      <c r="B7" s="193"/>
-      <c r="C7" s="182"/>
+    <row r="7" spans="2:7" ht="155.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="200"/>
+      <c r="C7" s="189"/>
       <c r="D7" s="101" t="s">
         <v>156</v>
       </c>
@@ -13180,13 +13972,13 @@
       <c r="F7" s="129"/>
       <c r="G7" s="104"/>
     </row>
-    <row r="8" spans="2:7" ht="99.75" customHeight="1">
-      <c r="B8" s="193"/>
-      <c r="C8" s="182"/>
-      <c r="D8" s="187" t="s">
+    <row r="8" spans="2:7" ht="99.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="200"/>
+      <c r="C8" s="189"/>
+      <c r="D8" s="194" t="s">
         <v>152</v>
       </c>
-      <c r="E8" s="184" t="s">
+      <c r="E8" s="191" t="s">
         <v>126</v>
       </c>
       <c r="F8" s="101" t="s">
@@ -13196,11 +13988,11 @@
         <v>164</v>
       </c>
     </row>
-    <row r="9" spans="2:7" ht="60" customHeight="1">
-      <c r="B9" s="193"/>
-      <c r="C9" s="182"/>
-      <c r="D9" s="188"/>
-      <c r="E9" s="185"/>
+    <row r="9" spans="2:7" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="200"/>
+      <c r="C9" s="189"/>
+      <c r="D9" s="195"/>
+      <c r="E9" s="192"/>
       <c r="F9" s="101" t="s">
         <v>148</v>
       </c>
@@ -13208,11 +14000,11 @@
         <v>157</v>
       </c>
     </row>
-    <row r="10" spans="2:7" ht="60" customHeight="1">
-      <c r="B10" s="193"/>
-      <c r="C10" s="182"/>
-      <c r="D10" s="188"/>
-      <c r="E10" s="185"/>
+    <row r="10" spans="2:7" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="200"/>
+      <c r="C10" s="189"/>
+      <c r="D10" s="195"/>
+      <c r="E10" s="192"/>
       <c r="F10" s="101" t="s">
         <v>137</v>
       </c>
@@ -13220,11 +14012,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="11" spans="2:7" ht="60" customHeight="1">
-      <c r="B11" s="193"/>
-      <c r="C11" s="182"/>
-      <c r="D11" s="188"/>
-      <c r="E11" s="185"/>
+    <row r="11" spans="2:7" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="200"/>
+      <c r="C11" s="189"/>
+      <c r="D11" s="195"/>
+      <c r="E11" s="192"/>
       <c r="F11" s="101" t="s">
         <v>136</v>
       </c>
@@ -13232,11 +14024,11 @@
         <v>149</v>
       </c>
     </row>
-    <row r="12" spans="2:7" ht="60" customHeight="1">
-      <c r="B12" s="193"/>
-      <c r="C12" s="182"/>
-      <c r="D12" s="188"/>
-      <c r="E12" s="185"/>
+    <row r="12" spans="2:7" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="200"/>
+      <c r="C12" s="189"/>
+      <c r="D12" s="195"/>
+      <c r="E12" s="192"/>
       <c r="F12" s="101" t="s">
         <v>135</v>
       </c>
@@ -13244,11 +14036,11 @@
         <v>160</v>
       </c>
     </row>
-    <row r="13" spans="2:7" ht="60" customHeight="1">
-      <c r="B13" s="194"/>
-      <c r="C13" s="183"/>
-      <c r="D13" s="189"/>
-      <c r="E13" s="186"/>
+    <row r="13" spans="2:7" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="201"/>
+      <c r="C13" s="190"/>
+      <c r="D13" s="196"/>
+      <c r="E13" s="193"/>
       <c r="F13" s="105" t="s">
         <v>133</v>
       </c>
@@ -13256,8 +14048,8 @@
         <v>134</v>
       </c>
     </row>
-    <row r="16" spans="2:7" ht="99" customHeight="1"/>
-    <row r="17" ht="138" customHeight="1"/>
+    <row r="16" spans="2:7" ht="99" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="17" ht="138" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="B2:B3"/>
@@ -13276,82 +14068,362 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{170671FC-7126-4F53-9577-31F7E194AC02}">
+  <dimension ref="A1:L15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9:D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="101" style="202" customWidth="1"/>
+    <col min="2" max="2" width="12.75" style="202" customWidth="1"/>
+    <col min="3" max="3" width="74.75" style="202" customWidth="1"/>
+    <col min="4" max="4" width="84.625" style="202" customWidth="1"/>
+    <col min="5" max="5" width="41.375" style="202" customWidth="1"/>
+    <col min="6" max="6" width="33.75" style="204" customWidth="1"/>
+    <col min="7" max="7" width="43.125" style="203" customWidth="1"/>
+    <col min="8" max="8" width="46.375" style="203" customWidth="1"/>
+    <col min="9" max="9" width="27.25" style="203" customWidth="1"/>
+    <col min="10" max="10" width="16.125" style="203" customWidth="1"/>
+    <col min="11" max="11" width="14" style="203" customWidth="1"/>
+    <col min="12" max="12" width="53.375" style="203" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="203" t="s">
+        <v>200</v>
+      </c>
+      <c r="B1" s="203"/>
+      <c r="C1" s="203"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="203" t="s">
+        <v>199</v>
+      </c>
+      <c r="B2" s="203"/>
+      <c r="C2" s="203"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="203" t="s">
+        <v>198</v>
+      </c>
+      <c r="B3" s="203"/>
+      <c r="C3" s="203"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="203" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" s="203"/>
+      <c r="C4" s="203"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="206" t="s">
+        <v>110</v>
+      </c>
+      <c r="B5" s="205" t="s">
+        <v>222</v>
+      </c>
+      <c r="C5" s="227" t="s">
+        <v>223</v>
+      </c>
+      <c r="D5" s="228" t="s">
+        <v>224</v>
+      </c>
+      <c r="E5" s="231" t="s">
+        <v>227</v>
+      </c>
+      <c r="F5" s="232"/>
+      <c r="G5" s="233"/>
+      <c r="H5" s="234"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="206"/>
+      <c r="B6" s="205"/>
+      <c r="C6" s="229"/>
+      <c r="D6" s="230" t="s">
+        <v>225</v>
+      </c>
+      <c r="E6" s="235" t="s">
+        <v>228</v>
+      </c>
+      <c r="F6" s="236" t="s">
+        <v>229</v>
+      </c>
+      <c r="G6" s="237" t="s">
+        <v>230</v>
+      </c>
+      <c r="H6" s="238" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="206"/>
+      <c r="B7" s="206" t="s">
+        <v>193</v>
+      </c>
+      <c r="C7" s="203" t="s">
+        <v>194</v>
+      </c>
+      <c r="D7" s="203"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="206"/>
+      <c r="B8" s="206"/>
+      <c r="C8" s="203" t="s">
+        <v>195</v>
+      </c>
+      <c r="D8" s="203"/>
+    </row>
+    <row r="9" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="206"/>
+      <c r="B9" s="206"/>
+      <c r="C9" s="206" t="s">
+        <v>196</v>
+      </c>
+      <c r="D9" s="207" t="s">
+        <v>197</v>
+      </c>
+      <c r="E9" s="207" t="s">
+        <v>215</v>
+      </c>
+      <c r="F9" s="208" t="s">
+        <v>208</v>
+      </c>
+      <c r="G9" s="209" t="s">
+        <v>209</v>
+      </c>
+      <c r="H9" s="210" t="s">
+        <v>201</v>
+      </c>
+      <c r="I9" s="209"/>
+      <c r="J9" s="209"/>
+      <c r="K9" s="209"/>
+      <c r="L9" s="211"/>
+    </row>
+    <row r="10" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="206"/>
+      <c r="B10" s="206"/>
+      <c r="C10" s="206"/>
+      <c r="D10" s="207"/>
+      <c r="E10" s="207"/>
+      <c r="F10" s="212"/>
+      <c r="G10" s="213" t="s">
+        <v>210</v>
+      </c>
+      <c r="H10" s="213" t="s">
+        <v>226</v>
+      </c>
+      <c r="I10" s="214" t="s">
+        <v>211</v>
+      </c>
+      <c r="J10" s="213" t="s">
+        <v>202</v>
+      </c>
+      <c r="K10" s="215" t="s">
+        <v>212</v>
+      </c>
+      <c r="L10" s="216" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" s="206"/>
+      <c r="B11" s="206"/>
+      <c r="C11" s="206"/>
+      <c r="D11" s="207"/>
+      <c r="E11" s="207"/>
+      <c r="F11" s="212"/>
+      <c r="G11" s="213"/>
+      <c r="H11" s="213"/>
+      <c r="I11" s="214"/>
+      <c r="J11" s="213"/>
+      <c r="K11" s="215" t="s">
+        <v>213</v>
+      </c>
+      <c r="L11" s="217" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" s="206"/>
+      <c r="B12" s="206"/>
+      <c r="C12" s="206"/>
+      <c r="D12" s="207"/>
+      <c r="E12" s="207"/>
+      <c r="F12" s="212"/>
+      <c r="G12" s="213"/>
+      <c r="H12" s="213"/>
+      <c r="I12" s="214"/>
+      <c r="J12" s="215" t="s">
+        <v>203</v>
+      </c>
+      <c r="K12" s="215"/>
+      <c r="L12" s="217" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" s="206"/>
+      <c r="B13" s="206"/>
+      <c r="C13" s="206"/>
+      <c r="D13" s="207"/>
+      <c r="E13" s="207"/>
+      <c r="F13" s="212"/>
+      <c r="G13" s="213"/>
+      <c r="H13" s="222" t="s">
+        <v>214</v>
+      </c>
+      <c r="I13" s="222" t="s">
+        <v>216</v>
+      </c>
+      <c r="J13" s="215"/>
+      <c r="K13" s="215" t="s">
+        <v>218</v>
+      </c>
+      <c r="L13" s="216" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="206"/>
+      <c r="B14" s="206"/>
+      <c r="C14" s="206"/>
+      <c r="D14" s="207"/>
+      <c r="E14" s="207"/>
+      <c r="F14" s="212"/>
+      <c r="G14" s="213"/>
+      <c r="H14" s="223"/>
+      <c r="I14" s="225"/>
+      <c r="J14" s="215"/>
+      <c r="K14" s="215" t="s">
+        <v>220</v>
+      </c>
+      <c r="L14" s="226" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" s="206"/>
+      <c r="B15" s="206"/>
+      <c r="C15" s="206"/>
+      <c r="D15" s="207"/>
+      <c r="E15" s="207"/>
+      <c r="F15" s="218"/>
+      <c r="G15" s="219"/>
+      <c r="H15" s="224"/>
+      <c r="I15" s="220" t="s">
+        <v>217</v>
+      </c>
+      <c r="J15" s="220"/>
+      <c r="K15" s="220"/>
+      <c r="L15" s="221" t="s">
+        <v>207</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="B7:B15"/>
+    <mergeCell ref="A5:A15"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="F9:F15"/>
+    <mergeCell ref="E9:E15"/>
+    <mergeCell ref="D9:D15"/>
+    <mergeCell ref="C9:C15"/>
+    <mergeCell ref="G10:G15"/>
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="H10:H12"/>
+    <mergeCell ref="I10:I12"/>
+    <mergeCell ref="H13:H15"/>
+    <mergeCell ref="I13:I14"/>
+  </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1315223-EA03-458B-929B-BCBCA8DFEC8C}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="144.1796875" customWidth="1"/>
-    <col min="2" max="2" width="101.1796875" customWidth="1"/>
+    <col min="1" max="1" width="144.125" customWidth="1"/>
+    <col min="2" max="2" width="101.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="99.5" customHeight="1">
-      <c r="A1" s="199" t="s">
+    <row r="1" spans="1:2" ht="99.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="135" t="s">
         <v>183</v>
       </c>
-      <c r="B1" s="200" t="s">
+      <c r="B1" s="136" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="50" customFormat="1" ht="20" customHeight="1">
-      <c r="A2" s="198" t="s">
+    <row r="2" spans="1:2" s="50" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="134" t="s">
         <v>186</v>
       </c>
-      <c r="B2" s="198"/>
+      <c r="B2" s="134"/>
     </row>
-    <row r="3" spans="1:2" ht="123.5" customHeight="1">
+    <row r="3" spans="1:2" ht="123.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>175</v>
       </c>
       <c r="B3" s="8"/>
     </row>
-    <row r="4" spans="1:2" ht="213" customHeight="1">
-      <c r="A4" s="195" t="s">
+    <row r="4" spans="1:2" ht="213" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="131" t="s">
         <v>187</v>
       </c>
-      <c r="B4" s="196" t="s">
+      <c r="B4" s="132" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="35" customHeight="1">
+    <row r="5" spans="1:2" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>176</v>
       </c>
       <c r="B5" s="8"/>
     </row>
-    <row r="6" spans="1:2" ht="80" customHeight="1">
+    <row r="6" spans="1:2" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>181</v>
       </c>
       <c r="B6" s="8"/>
     </row>
-    <row r="7" spans="1:2" s="50" customFormat="1" ht="60" customHeight="1">
-      <c r="A7" s="198" t="s">
+    <row r="7" spans="1:2" s="50" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="134" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="201" t="s">
+      <c r="B7" s="137" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="192.5" customHeight="1">
-      <c r="A8" s="197" t="s">
+    <row r="8" spans="1:2" ht="192.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="133" t="s">
         <v>180</v>
       </c>
-      <c r="B8" s="197" t="s">
+      <c r="B8" s="133" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="32">
+    <row r="9" spans="1:2" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
         <v>182</v>
       </c>
       <c r="B9" s="8"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
BMW_SecOc add printSecOc messages in Key-ID Tab
</commit_message>
<xml_diff>
--- a/BMW_SecOc.xlsx
+++ b/BMW_SecOc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git_XuhuaRepo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98C5642B-08C2-43DB-A481-3541F06A36E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F16A1949-0596-491B-B2EF-8033B9ADB236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-8640" windowWidth="38640" windowHeight="21240" activeTab="6" xr2:uid="{EE3554E5-5B85-4F6F-95D2-24E55C4E92D2}"/>
+    <workbookView xWindow="28680" yWindow="-8640" windowWidth="38640" windowHeight="21240" activeTab="5" xr2:uid="{EE3554E5-5B85-4F6F-95D2-24E55C4E92D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Code" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="250">
   <si>
     <t>DsBusCustomCode_onPduFeatureExecutionPrivate(pduFeatureHandle)</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -9806,21 +9806,451 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>CollectStaticPduProperties</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CollectStaticPduPropertiesDuringRuntimeForAllSecOCMsgs</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CollectStaticPduPropertiesDuringRuntimeForAllSecOCMsgsPerCluster</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">for (unsigned int i = 0; i &lt; filteredSecOCMsgs-&gt;itemCount; i++) {
-    pduFeatData = (UserCode_FeatureData *)GetById(filteredSecOCMsgs, i);
+    <t>DsBusCustomCode_onPduFeatureExecutionPrivate</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>"internal"</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>dataIdExists</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>!dataIdExists</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>"external"</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>"DataID: %d is not found in dataID_file."</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>"DataID is not defined in cluster database."</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>"Key-id for Message '%s' is missing"</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiBold"/>
+        <family val="3"/>
+      </rPr>
+      <t>DsBusCustomCodeSecuredIPdu_getKeyId(securedIPdu_PduHandle, &amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Cascadia Mono SemiBold"/>
+        <family val="3"/>
+      </rPr>
+      <t>keyId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiBold"/>
+        <family val="3"/>
+      </rPr>
+      <t>);
+DsBusCustomCodeSecuredIPdu_getDataId(securedIPdu_PduHandle, &amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Cascadia Mono SemiBold"/>
+        <family val="3"/>
+      </rPr>
+      <t>dataId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiBold"/>
+        <family val="3"/>
+      </rPr>
+      <t>);</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Cascadia Mono SemiBold"/>
+        <family val="3"/>
+      </rPr>
+      <t>keyId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono Light"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> != 0</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Cascadia Mono SemiBold"/>
+        <family val="3"/>
+      </rPr>
+      <t>keyId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono Light"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> == 0</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFEE0000"/>
+        <rFont val="Cascadia Mono SemiBold"/>
+        <family val="3"/>
+      </rPr>
+      <t>keyId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiBold"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> = GetKeyId(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFEE0000"/>
+        <rFont val="Cascadia Mono SemiBold"/>
+        <family val="3"/>
+      </rPr>
+      <t>dataId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiBold"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFEE0000"/>
+        <rFont val="Cascadia Mono SemiBold"/>
+        <family val="3"/>
+      </rPr>
+      <t>keyId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono Light"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> &gt; 0</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFEE0000"/>
+        <rFont val="Cascadia Mono SemiBold"/>
+        <family val="3"/>
+      </rPr>
+      <t>keyId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono Light"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> == 0</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>if (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFEE0000"/>
+        <rFont val="Cascadia Mono SemiBold"/>
+        <family val="3"/>
+      </rPr>
+      <t>keyId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono Light"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> &lt;= 0)</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">rtnVal = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono SemiBold"/>
+        <family val="3"/>
+      </rPr>
+      <t>DsBusCustomCode_collectStaticPduPropertiesDuringRuntimeEx(pduFeatData)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono Light"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">;
+if (rtnVal != E_OK){
+    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Cascadia Mono Light"/>
+        <family val="3"/>
+      </rPr>
+      <t>"Last error message refers to 'SecuredIPdu_Name'"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono Light"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">
+}</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>if(IsAnyCounterMessage)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>if!(IsAnyCounterMessage)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFEE0000"/>
+        <rFont val="Cascadia Mono SemiBold"/>
+        <family val="3"/>
+      </rPr>
+      <t>keyId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono Light"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> != -1</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>"SecOCSetup"</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>keyId == -1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>"For Rx-Counter-Message '%s' key-id is missing. "
+"For Tx-Counter-Message '%s' key-id is missing. "</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>mdlStart</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>InitDataKeyIdMapping</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>(int)(*inDataKeyIdPairsDataPtr[0])==0</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>(int)(*inDataKeyIdPairsDataPtr[0])!=0</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>if (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="8"/>
+        <rFont val="Cascadia Mono SemiBold"/>
+        <family val="3"/>
+      </rPr>
+      <t>externalKeyIdFileExists</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono Light"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>externalKeyIdFileExists == 0</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>externalKeyIdFileExists == 1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>InitKeyIdsStruct</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SetKeyId(Const_dataId, Const_keyId)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>g_keyids[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFEE0000"/>
+        <rFont val="Cascadia Mono SemiBold"/>
+        <family val="3"/>
+      </rPr>
+      <t>dataId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono Light"/>
+        <family val="3"/>
+      </rPr>
+      <t>].</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFEE0000"/>
+        <rFont val="Cascadia Code SemiBold"/>
+        <family val="3"/>
+      </rPr>
+      <t>keyId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono Light"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> = (uint32)keyId</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>CollectStaticPduProperties
+CollectStaticPduPropertiesDuringRuntimeForAllSecOCMsgs
+CollectStaticPduPropertiesDuringRuntimeForAllSecOCMsgsPerCluster</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>PrintCollectedPduProperties
+PrintListOfAllSecOCMsgs</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>for (unsigned int i = 0; i &lt; filteredSecOCMsgs-&gt;itemCount; i++) {
+    pduFeatData = (UserCode_FeatureData *)GetById(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF00FF"/>
+        <rFont val="Cascadia Code SemiBold"/>
+        <family val="3"/>
+      </rPr>
+      <t>filteredSecOCMsgs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono Light"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, i);
     </t>
     </r>
     <r>
@@ -9886,103 +10316,267 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>DsBusCustomCode_onPduFeatureExecutionPrivate</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>g_DsBusCustomCode_onPduFeatureExecutionPrivateFunc = DsBusCustomCode_onPduFeatureExecutionPrivate</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">DsBusCustomCode_onPduFeatureExecution(DsBusCustomCodePduFeatureHandle pduFeatureHandle) </t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>"internal"</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>dataIdExists</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>!dataIdExists</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>"external"</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>"DataID: %d is not found in dataID_file."</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>"DataID is not defined in cluster database."</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>"Key-id for Message '%s' is missing"</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
+    <r>
+      <t>GetFilteredClusterAgentsList</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t>（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF00FF"/>
         <rFont val="Cascadia Mono SemiBold"/>
         <family val="3"/>
       </rPr>
-      <t>DsBusCustomCodeSecuredIPdu_getKeyId(securedIPdu_PduHandle, &amp;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
+      <t>filteredClusterList</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono Light"/>
+        <family val="3"/>
+      </rPr>
+      <t>, isClusterSlBlkAssigned</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>DsBusCustomCode_onPduFeatureExecution</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>PrintListOfAllSecOCMsgsPerCluster
+(clusterAgent-&gt;Ident, "    ", "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFEE0000"/>
+        <rFont val="Cascadia Mono Light"/>
+        <family val="3"/>
+      </rPr>
+      <t>error</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono Light"/>
+        <family val="3"/>
+      </rPr>
+      <t>")</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>PrintListOfAllSecOCMsgsPerCluster
+(clusterAgent-&gt;Ident, NULL, "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Cascadia Mono Light"/>
+        <family val="3"/>
+      </rPr>
+      <t>info</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono Light"/>
+        <family val="3"/>
+      </rPr>
+      <t>")</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>for (unsigned int i = 0; i &lt; DQueueSize(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF00FF"/>
         <rFont val="Cascadia Mono SemiBold"/>
         <family val="3"/>
       </rPr>
-      <t>keyId</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
+      <t>filteredClusterList</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono Light"/>
+        <family val="3"/>
+      </rPr>
+      <t>); i++) {
+    clusterAgent = (ClusterAgentStruct*)GetById(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF00FF"/>
         <rFont val="Cascadia Mono SemiBold"/>
         <family val="3"/>
       </rPr>
-      <t>);
-DsBusCustomCodeSecuredIPdu_getDataId(securedIPdu_PduHandle, &amp;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
+      <t>filteredClusterList</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono Light"/>
+        <family val="3"/>
+      </rPr>
+      <t>, i)</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>GetClusterAgentById
+((unsigned char)clusterId, &amp;clusterAgent)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">if (clusterAgent != NULL)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Cascadia Mono Light"/>
+        <family val="3"/>
+      </rPr>
+      <t>"List of all SecOC-Messages of cluster 'clusterAgent-&gt;Name 'found:"</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">isClusterSlBlkAssigned = TRUE
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono Light"/>
+        <family val="3"/>
+      </rPr>
+      <t>//Print Messages with clusters assigned to SL-Blocks</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>isClusterSlBlkAssigned = FALSE
+//Print Messages with missing cluster to SL-Blocks assignment</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">if (clusterAgent == NULL)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Cascadia Mono Light"/>
+        <family val="3"/>
+      </rPr>
+      <t>"No SecOC-Messages assigned to cluster clusterAgent-&gt;Name found")</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>GetFilteredListOfConfiguredSecOCMsgs
+(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFEB65BE"/>
         <rFont val="Cascadia Mono SemiBold"/>
         <family val="3"/>
       </rPr>
-      <t>dataId</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
+      <t>filteredSecOCMsgs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono Light"/>
+        <family val="3"/>
+      </rPr>
+      <t>, clusterId,"rx", ARG_NA)</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>GetFilteredListOfConfiguredSecOCMsgs
+(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFEB65BE"/>
         <rFont val="Cascadia Mono SemiBold"/>
         <family val="3"/>
       </rPr>
-      <t>);</t>
-    </r>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
+      <t>filteredSecOCMsgs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono Light"/>
+        <family val="3"/>
+      </rPr>
+      <t>, clusterId,"tx", ARG_NA)</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>GetFilteredListOfConfiguredSecOCMsgs
+(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFEB65BE"/>
         <rFont val="Cascadia Mono SemiBold"/>
         <family val="3"/>
       </rPr>
-      <t>keyId</t>
+      <t>filteredSecOCMsgs</t>
     </r>
     <r>
       <rPr>
@@ -9991,19 +10585,41 @@
         <rFont val="Cascadia Mono Light"/>
         <family val="3"/>
       </rPr>
-      <t xml:space="preserve"> != 0</t>
-    </r>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
+      <t xml:space="preserve">, clusterId,"rx", </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFEE0000"/>
+        <rFont val="Cascadia Mono Light"/>
+        <family val="3"/>
+      </rPr>
+      <t>errorFreePropCollected</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono Light"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>GetFilteredListOfConfiguredSecOCMsgs
+(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFEB65BE"/>
         <rFont val="Cascadia Mono SemiBold"/>
         <family val="3"/>
       </rPr>
-      <t>keyId</t>
+      <t>filteredSecOCMsgs</t>
     </r>
     <r>
       <rPr>
@@ -10012,79 +10628,41 @@
         <rFont val="Cascadia Mono Light"/>
         <family val="3"/>
       </rPr>
-      <t xml:space="preserve"> == 0</t>
-    </r>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
+      <t xml:space="preserve">, clusterId,"tx", </t>
+    </r>
     <r>
       <rPr>
         <sz val="11"/>
         <color rgb="FFEE0000"/>
-        <rFont val="Cascadia Mono SemiBold"/>
-        <family val="3"/>
-      </rPr>
-      <t>keyId</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Cascadia Mono SemiBold"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> = GetKeyId(</t>
+        <rFont val="Cascadia Mono Light"/>
+        <family val="3"/>
+      </rPr>
+      <t>errorFreePropCollected</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono Light"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>PrintMsgList
+(</t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
         <color rgb="FFEE0000"/>
-        <rFont val="Cascadia Mono SemiBold"/>
-        <family val="3"/>
-      </rPr>
-      <t>dataId</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Cascadia Mono SemiBold"/>
-        <family val="3"/>
-      </rPr>
-      <t>)</t>
-    </r>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFEE0000"/>
-        <rFont val="Cascadia Mono SemiBold"/>
-        <family val="3"/>
-      </rPr>
-      <t>keyId</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
         <rFont val="Cascadia Mono Light"/>
         <family val="3"/>
       </rPr>
-      <t xml:space="preserve"> &gt; 0</t>
-    </r>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFEE0000"/>
-        <rFont val="Cascadia Mono SemiBold"/>
-        <family val="3"/>
-      </rPr>
-      <t>keyId</t>
+      <t>error</t>
     </r>
     <r>
       <rPr>
@@ -10093,22 +10671,16 @@
         <rFont val="Cascadia Mono Light"/>
         <family val="3"/>
       </rPr>
-      <t xml:space="preserve"> == 0</t>
-    </r>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>if (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFEE0000"/>
-        <rFont val="Cascadia Mono SemiBold"/>
-        <family val="3"/>
-      </rPr>
-      <t>keyId</t>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFEB65BE"/>
+        <rFont val="Cascadia Code SemiBold"/>
+        <family val="3"/>
+      </rPr>
+      <t>filteredSecOCMsgs</t>
     </r>
     <r>
       <rPr>
@@ -10117,42 +10689,88 @@
         <rFont val="Cascadia Mono Light"/>
         <family val="3"/>
       </rPr>
-      <t xml:space="preserve"> &lt;= 0)</t>
-    </r>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">rtnVal = </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Cascadia Mono SemiBold"/>
-        <family val="3"/>
-      </rPr>
-      <t>DsBusCustomCode_collectStaticPduPropertiesDuringRuntimeEx(pduFeatData)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
+      <t>, "Rx/Tx")</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>PrintMsgList
+(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
         <rFont val="Cascadia Mono Light"/>
         <family val="3"/>
       </rPr>
-      <t xml:space="preserve">;
-if (rtnVal != E_OK){
-    </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
+      <t>info</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
         <rFont val="Cascadia Mono Light"/>
         <family val="3"/>
       </rPr>
-      <t>"Last error message refers to 'SecuredIPdu_Name'"</t>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFEB65BE"/>
+        <rFont val="Cascadia Code SemiBold"/>
+        <family val="3"/>
+      </rPr>
+      <t>filteredSecOCMsgs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono Light"/>
+        <family val="3"/>
+      </rPr>
+      <t>, "Rx/Tx")</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>"Tx/Rx-Messages configured as SecOC (secured-PDU-names) are:"</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">for (unsigned int i = 0; i &lt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFEB65BE"/>
+        <rFont val="Cascadia Code SemiBold"/>
+        <family val="3"/>
+      </rPr>
+      <t>filteredSecOCMsgs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono Light"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">-&gt;itemCount; i++) {
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Cascadia Mono Light"/>
+        <family val="3"/>
+      </rPr>
+      <t>"shortPduName (Key-Id=%d) (Key-Id-Source: %s)"</t>
     </r>
     <r>
       <rPr>
@@ -10167,22 +10785,39 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>if(IsAnyCounterMessage)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>if!(IsAnyCounterMessage)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono Light"/>
+        <family val="3"/>
+      </rPr>
+      <t>if (clusterAgent != NULL)</t>
+    </r>
     <r>
       <rPr>
         <sz val="11"/>
         <color rgb="FFEE0000"/>
+        <rFont val="Cascadia Mono Light"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">
+"error", "%sList of faulty Tx/Rx-SecOC-Messages (not properly initialized):"</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">for (unsigned int i = 0; i &lt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFEB65BE"/>
         <rFont val="Cascadia Mono SemiBold"/>
         <family val="3"/>
       </rPr>
-      <t>keyId</t>
+      <t>filteredSecOCMsgs</t>
     </r>
     <r>
       <rPr>
@@ -10191,109 +10826,54 @@
         <rFont val="Cascadia Mono Light"/>
         <family val="3"/>
       </rPr>
-      <t xml:space="preserve"> != -1</t>
-    </r>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>"SecOCSetup"</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>keyId == -1</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>"For Rx-Counter-Message '%s' key-id is missing. "
-"For Tx-Counter-Message '%s' key-id is missing. "</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>mdlStart</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>InitDataKeyIdMapping</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>(int)(*inDataKeyIdPairsDataPtr[0])==0</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>(int)(*inDataKeyIdPairsDataPtr[0])!=0</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>if (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="8"/>
-        <rFont val="Cascadia Mono SemiBold"/>
-        <family val="3"/>
-      </rPr>
-      <t>externalKeyIdFileExists</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
+      <t xml:space="preserve">-&gt;itemCount; i++) {
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFEE0000"/>
         <rFont val="Cascadia Mono Light"/>
         <family val="3"/>
       </rPr>
-      <t>)</t>
-    </r>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>externalKeyIdFileExists == 0</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>externalKeyIdFileExists == 1</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>InitKeyIdsStruct</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>SetKeyId(Const_dataId, Const_keyId)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>g_keyids[</t>
+      <t xml:space="preserve">"shortPduName (Key-Id=%d) (Key-Id-Source: %s)"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono Light"/>
+        <family val="3"/>
+      </rPr>
+      <t>}</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">"error", "List of messages linked to clusters with missing Simulink-block assignment:"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Mono Light"/>
+        <family val="3"/>
+      </rPr>
+      <t>for (unsigned int i = 0; i &lt; DQueueSize(filteredClusterList); i++) {
+    clusterAgent = (ClusterAgentStruct*)GetById(filteredClusterList, i);
+    PrintListOfAllSecOCMsgsPerCluster(clusterAgent-&gt;Ident, "    ", "</t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
         <color rgb="FFEE0000"/>
-        <rFont val="Cascadia Mono SemiBold"/>
-        <family val="3"/>
-      </rPr>
-      <t>dataId</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
         <rFont val="Cascadia Mono Light"/>
         <family val="3"/>
       </rPr>
-      <t>].</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFEE0000"/>
-        <rFont val="Cascadia Code SemiBold"/>
-        <family val="3"/>
-      </rPr>
-      <t>keyId</t>
+      <t>error</t>
     </r>
     <r>
       <rPr>
@@ -10302,7 +10882,8 @@
         <rFont val="Cascadia Mono Light"/>
         <family val="3"/>
       </rPr>
-      <t xml:space="preserve"> = (uint32)keyId</t>
+      <t>");
+}</t>
     </r>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -10311,7 +10892,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="50" x14ac:knownFonts="1">
+  <fonts count="56" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -10650,6 +11231,44 @@
       <name val="Cascadia Mono SemiBold"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF00FF"/>
+      <name val="Cascadia Mono SemiBold"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF00FF"/>
+      <name val="Cascadia Mono SemiBold"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Cascadia Mono Light"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFEB65BE"/>
+      <name val="Cascadia Mono SemiBold"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFEB65BE"/>
+      <name val="Cascadia Code SemiBold"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="18">
     <fill>
@@ -10755,7 +11374,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="67">
+  <borders count="68">
     <border>
       <left/>
       <right/>
@@ -11645,23 +12264,36 @@
       <diagonal/>
     </border>
     <border>
-      <left style="hair">
+      <left style="dashed">
         <color auto="1"/>
       </left>
       <right style="hair">
         <color auto="1"/>
       </right>
-      <top/>
-      <bottom style="dashed">
-        <color auto="1"/>
-      </bottom>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="dashed">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="239">
+  <cellXfs count="251">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -12036,6 +12668,51 @@
     <xf numFmtId="0" fontId="30" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="42" fillId="16" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="16" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="16" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="16" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="16" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="16" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="16" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="16" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="16" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="49" fillId="16" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="16" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="42" fillId="16" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -12228,110 +12905,101 @@
     <xf numFmtId="0" fontId="5" fillId="15" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="25" fillId="16" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="16" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="16" borderId="58" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="16" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="16" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="16" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="16" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="16" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="16" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="16" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="16" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="14" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="16" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="14" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="14" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="14" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="16" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="14" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="14" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="16" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="45" fillId="14" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="14" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="14" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="14" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="16" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="16" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="16" borderId="62" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="16" borderId="62" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="16" borderId="63" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="14" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="16" borderId="64" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="16" borderId="64" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="16" borderId="65" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="16" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="16" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="16" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="16" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="16" borderId="62" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="47" fillId="14" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="16" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="16" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="42" fillId="16" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="16" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="16" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="16" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="42" fillId="16" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="16" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="42" fillId="14" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -12341,9 +13009,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFEB65BE"/>
       <color rgb="FFCFAFE7"/>
       <color rgb="FFFF00FF"/>
-      <color rgb="FFEB65BE"/>
       <color rgb="FFFF5050"/>
       <color rgb="FFFDBC53"/>
     </mruColors>
@@ -12683,7 +13351,7 @@
       <c r="B2" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="146" t="s">
+      <c r="C2" s="163" t="s">
         <v>109</v>
       </c>
     </row>
@@ -12694,7 +13362,7 @@
       <c r="B3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="147"/>
+      <c r="C3" s="164"/>
     </row>
     <row r="4" spans="1:3" ht="386.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
@@ -12703,7 +13371,7 @@
       <c r="B4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="148"/>
+      <c r="C4" s="165"/>
     </row>
     <row r="5" spans="1:3" ht="200.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
@@ -12736,11 +13404,11 @@
       <c r="C8" s="16"/>
     </row>
     <row r="9" spans="1:3" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="154" t="s">
+      <c r="A9" s="171" t="s">
         <v>140</v>
       </c>
-      <c r="B9" s="154"/>
-      <c r="C9" s="155"/>
+      <c r="B9" s="171"/>
+      <c r="C9" s="172"/>
     </row>
     <row r="10" spans="1:3" ht="287.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="95" t="s">
@@ -12749,7 +13417,7 @@
       <c r="B10" s="96" t="s">
         <v>74</v>
       </c>
-      <c r="C10" s="149" t="s">
+      <c r="C10" s="166" t="s">
         <v>8</v>
       </c>
     </row>
@@ -12760,23 +13428,23 @@
       <c r="B11" s="96" t="s">
         <v>141</v>
       </c>
-      <c r="C11" s="150"/>
+      <c r="C11" s="167"/>
     </row>
     <row r="12" spans="1:3" ht="257.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="152" t="s">
+      <c r="A12" s="169" t="s">
         <v>142</v>
       </c>
       <c r="B12" s="96" t="s">
         <v>80</v>
       </c>
-      <c r="C12" s="150"/>
+      <c r="C12" s="167"/>
     </row>
     <row r="13" spans="1:3" ht="120.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="153"/>
+      <c r="A13" s="170"/>
       <c r="B13" s="96" t="s">
         <v>79</v>
       </c>
-      <c r="C13" s="151"/>
+      <c r="C13" s="168"/>
     </row>
     <row r="14" spans="1:3" ht="157.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="98" t="s">
@@ -12785,7 +13453,7 @@
       <c r="B14" s="96" t="s">
         <v>144</v>
       </c>
-      <c r="C14" s="149" t="s">
+      <c r="C14" s="166" t="s">
         <v>147</v>
       </c>
     </row>
@@ -12796,7 +13464,7 @@
       <c r="B15" s="96" t="s">
         <v>146</v>
       </c>
-      <c r="C15" s="151"/>
+      <c r="C15" s="168"/>
     </row>
     <row r="16" spans="1:3" ht="378.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
@@ -12805,7 +13473,7 @@
       <c r="B16" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="C16" s="146"/>
+      <c r="C16" s="163"/>
     </row>
     <row r="17" spans="1:3" ht="110.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
@@ -12814,7 +13482,7 @@
       <c r="B17" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="147"/>
+      <c r="C17" s="164"/>
     </row>
     <row r="18" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="43" t="s">
@@ -12841,7 +13509,7 @@
       <c r="B20" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="C20" s="143" t="s">
+      <c r="C20" s="160" t="s">
         <v>73</v>
       </c>
     </row>
@@ -12850,7 +13518,7 @@
         <v>172</v>
       </c>
       <c r="B21" s="132"/>
-      <c r="C21" s="144"/>
+      <c r="C21" s="161"/>
     </row>
     <row r="22" spans="1:3" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
@@ -12859,7 +13527,7 @@
       <c r="B22" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C22" s="144"/>
+      <c r="C22" s="161"/>
     </row>
     <row r="23" spans="1:3" ht="370.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
@@ -12868,14 +13536,14 @@
       <c r="B23" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C23" s="145"/>
+      <c r="C23" s="162"/>
     </row>
     <row r="24" spans="1:3" ht="78.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
         <v>10</v>
       </c>
       <c r="B24" s="4"/>
-      <c r="C24" s="142" t="s">
+      <c r="C24" s="159" t="s">
         <v>71</v>
       </c>
     </row>
@@ -12884,7 +13552,7 @@
         <v>11</v>
       </c>
       <c r="B25" s="4"/>
-      <c r="C25" s="142"/>
+      <c r="C25" s="159"/>
     </row>
     <row r="26" spans="1:3" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
@@ -12893,7 +13561,7 @@
       <c r="B26" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="142"/>
+      <c r="C26" s="159"/>
     </row>
     <row r="27" spans="1:3" ht="242.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="10" t="s">
@@ -12902,35 +13570,35 @@
       <c r="B27" s="10" t="s">
         <v>184</v>
       </c>
-      <c r="C27" s="142"/>
+      <c r="C27" s="159"/>
     </row>
     <row r="28" spans="1:3" ht="110.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
         <v>13</v>
       </c>
       <c r="B28" s="12"/>
-      <c r="C28" s="142"/>
+      <c r="C28" s="159"/>
     </row>
     <row r="29" spans="1:3" ht="224.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="12" t="s">
         <v>60</v>
       </c>
       <c r="B29" s="12"/>
-      <c r="C29" s="142"/>
+      <c r="C29" s="159"/>
     </row>
     <row r="30" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="133" t="s">
         <v>173</v>
       </c>
       <c r="B30" s="133"/>
-      <c r="C30" s="142"/>
+      <c r="C30" s="159"/>
     </row>
     <row r="31" spans="1:3" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="12" t="s">
         <v>98</v>
       </c>
       <c r="B31" s="12"/>
-      <c r="C31" s="139"/>
+      <c r="C31" s="156"/>
     </row>
     <row r="32" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="43" t="s">
@@ -12946,7 +13614,7 @@
       <c r="B33" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="C33" s="138" t="s">
+      <c r="C33" s="155" t="s">
         <v>72</v>
       </c>
     </row>
@@ -12957,32 +13625,32 @@
       <c r="B34" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="C34" s="139"/>
+      <c r="C34" s="156"/>
     </row>
     <row r="35" spans="1:3" ht="234.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="140" t="s">
+      <c r="A35" s="157" t="s">
         <v>65</v>
       </c>
       <c r="B35" s="49" t="s">
         <v>169</v>
       </c>
-      <c r="C35" s="138" t="s">
+      <c r="C35" s="155" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="215.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="141"/>
+      <c r="A36" s="158"/>
       <c r="B36" s="12" t="s">
         <v>171</v>
       </c>
-      <c r="C36" s="142"/>
+      <c r="C36" s="159"/>
     </row>
     <row r="37" spans="1:3" ht="297.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="141"/>
+      <c r="A37" s="158"/>
       <c r="B37" s="12" t="s">
         <v>170</v>
       </c>
-      <c r="C37" s="142"/>
+      <c r="C37" s="159"/>
     </row>
     <row r="38" spans="1:3" ht="135.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="12" t="s">
@@ -12991,7 +13659,7 @@
       <c r="B38" s="12" t="s">
         <v>190</v>
       </c>
-      <c r="C38" s="139"/>
+      <c r="C38" s="156"/>
     </row>
     <row r="39" spans="1:3" ht="393.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="12" t="s">
@@ -13040,7 +13708,7 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="156" t="s">
+      <c r="B3" s="173" t="s">
         <v>109</v>
       </c>
       <c r="C3" s="90" t="s">
@@ -13048,7 +13716,7 @@
       </c>
     </row>
     <row r="4" spans="2:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="158"/>
+      <c r="B4" s="175"/>
       <c r="C4" s="90" t="s">
         <v>114</v>
       </c>
@@ -13060,7 +13728,7 @@
       <c r="C5" s="91"/>
     </row>
     <row r="6" spans="2:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="156" t="s">
+      <c r="B6" s="173" t="s">
         <v>110</v>
       </c>
       <c r="C6" s="90" t="s">
@@ -13068,19 +13736,19 @@
       </c>
     </row>
     <row r="7" spans="2:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="157"/>
+      <c r="B7" s="174"/>
       <c r="C7" s="90" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="157"/>
+      <c r="B8" s="174"/>
       <c r="C8" s="90" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="9" spans="2:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="158"/>
+      <c r="B9" s="175"/>
       <c r="C9" s="90" t="s">
         <v>114</v>
       </c>
@@ -13098,7 +13766,7 @@
       <c r="C11" s="91"/>
     </row>
     <row r="12" spans="2:3" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="159" t="s">
+      <c r="B12" s="176" t="s">
         <v>71</v>
       </c>
       <c r="C12" s="92" t="s">
@@ -13106,7 +13774,7 @@
       </c>
     </row>
     <row r="13" spans="2:3" ht="80.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="160"/>
+      <c r="B13" s="177"/>
       <c r="C13" s="92" t="s">
         <v>121</v>
       </c>
@@ -13165,25 +13833,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="203.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="161" t="s">
+      <c r="A1" s="178" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="168" t="s">
+      <c r="B1" s="185" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="167" t="s">
+      <c r="C1" s="184" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="167" t="s">
+      <c r="D1" s="184" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="167" t="s">
+      <c r="E1" s="184" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="167" t="s">
+      <c r="F1" s="184" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="167" t="s">
+      <c r="G1" s="184" t="s">
         <v>45</v>
       </c>
       <c r="H1" s="108" t="s">
@@ -13197,13 +13865,13 @@
       <c r="L1" s="109"/>
     </row>
     <row r="2" spans="1:12" ht="287.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="162"/>
-      <c r="B2" s="164"/>
-      <c r="C2" s="166"/>
-      <c r="D2" s="166"/>
-      <c r="E2" s="166"/>
-      <c r="F2" s="166"/>
-      <c r="G2" s="166"/>
+      <c r="A2" s="179"/>
+      <c r="B2" s="181"/>
+      <c r="C2" s="183"/>
+      <c r="D2" s="183"/>
+      <c r="E2" s="183"/>
+      <c r="F2" s="183"/>
+      <c r="G2" s="183"/>
       <c r="H2" s="110" t="s">
         <v>41</v>
       </c>
@@ -13219,14 +13887,14 @@
       <c r="L2" s="112"/>
     </row>
     <row r="3" spans="1:12" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="162"/>
-      <c r="B3" s="164"/>
-      <c r="C3" s="166"/>
-      <c r="D3" s="166"/>
-      <c r="E3" s="166" t="s">
+      <c r="A3" s="179"/>
+      <c r="B3" s="181"/>
+      <c r="C3" s="183"/>
+      <c r="D3" s="183"/>
+      <c r="E3" s="183" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="169" t="s">
+      <c r="F3" s="186" t="s">
         <v>33</v>
       </c>
       <c r="G3" s="110" t="s">
@@ -13239,16 +13907,16 @@
       <c r="L3" s="112"/>
     </row>
     <row r="4" spans="1:12" ht="233.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="162"/>
-      <c r="B4" s="164"/>
-      <c r="C4" s="166"/>
-      <c r="D4" s="166"/>
-      <c r="E4" s="166"/>
-      <c r="F4" s="169"/>
-      <c r="G4" s="166" t="s">
+      <c r="A4" s="179"/>
+      <c r="B4" s="181"/>
+      <c r="C4" s="183"/>
+      <c r="D4" s="183"/>
+      <c r="E4" s="183"/>
+      <c r="F4" s="186"/>
+      <c r="G4" s="183" t="s">
         <v>35</v>
       </c>
-      <c r="H4" s="166" t="s">
+      <c r="H4" s="183" t="s">
         <v>81</v>
       </c>
       <c r="I4" s="111" t="s">
@@ -13261,14 +13929,14 @@
       <c r="L4" s="112"/>
     </row>
     <row r="5" spans="1:12" ht="113.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="162"/>
-      <c r="B5" s="164"/>
-      <c r="C5" s="166"/>
-      <c r="D5" s="166"/>
-      <c r="E5" s="166"/>
-      <c r="F5" s="169"/>
-      <c r="G5" s="166"/>
-      <c r="H5" s="166"/>
+      <c r="A5" s="179"/>
+      <c r="B5" s="181"/>
+      <c r="C5" s="183"/>
+      <c r="D5" s="183"/>
+      <c r="E5" s="183"/>
+      <c r="F5" s="186"/>
+      <c r="G5" s="183"/>
+      <c r="H5" s="183"/>
       <c r="I5" s="111" t="s">
         <v>82</v>
       </c>
@@ -13283,10 +13951,10 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="160.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="162"/>
-      <c r="B6" s="164"/>
-      <c r="C6" s="166"/>
-      <c r="D6" s="166"/>
+      <c r="A6" s="179"/>
+      <c r="B6" s="181"/>
+      <c r="C6" s="183"/>
+      <c r="D6" s="183"/>
       <c r="E6" s="110" t="s">
         <v>32</v>
       </c>
@@ -13299,8 +13967,8 @@
       <c r="L6" s="112"/>
     </row>
     <row r="7" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="162"/>
-      <c r="B7" s="164" t="s">
+      <c r="A7" s="179"/>
+      <c r="B7" s="181" t="s">
         <v>38</v>
       </c>
       <c r="C7" s="113" t="s">
@@ -13317,8 +13985,8 @@
       <c r="L7" s="112"/>
     </row>
     <row r="8" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="162"/>
-      <c r="B8" s="164"/>
+      <c r="A8" s="179"/>
+      <c r="B8" s="181"/>
       <c r="C8" s="113" t="s">
         <v>40</v>
       </c>
@@ -13333,8 +14001,8 @@
       <c r="L8" s="112"/>
     </row>
     <row r="9" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="162"/>
-      <c r="B9" s="164"/>
+      <c r="A9" s="179"/>
+      <c r="B9" s="181"/>
       <c r="C9" s="113" t="s">
         <v>75</v>
       </c>
@@ -13349,8 +14017,8 @@
       <c r="L9" s="112"/>
     </row>
     <row r="10" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="162"/>
-      <c r="B10" s="164"/>
+      <c r="A10" s="179"/>
+      <c r="B10" s="181"/>
       <c r="C10" s="113" t="s">
         <v>76</v>
       </c>
@@ -13365,8 +14033,8 @@
       <c r="L10" s="112"/>
     </row>
     <row r="11" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="162"/>
-      <c r="B11" s="170" t="s">
+      <c r="A11" s="179"/>
+      <c r="B11" s="187" t="s">
         <v>67</v>
       </c>
       <c r="C11" s="14" t="s">
@@ -13383,8 +14051,8 @@
       <c r="L11" s="112"/>
     </row>
     <row r="12" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="162"/>
-      <c r="B12" s="171"/>
+      <c r="A12" s="179"/>
+      <c r="B12" s="188"/>
       <c r="C12" s="113" t="s">
         <v>166</v>
       </c>
@@ -13399,8 +14067,8 @@
       <c r="L12" s="112"/>
     </row>
     <row r="13" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="162"/>
-      <c r="B13" s="172"/>
+      <c r="A13" s="179"/>
+      <c r="B13" s="189"/>
       <c r="C13" s="113" t="s">
         <v>167</v>
       </c>
@@ -13415,8 +14083,8 @@
       <c r="L13" s="112"/>
     </row>
     <row r="14" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="162"/>
-      <c r="B14" s="170" t="s">
+      <c r="A14" s="179"/>
+      <c r="B14" s="187" t="s">
         <v>69</v>
       </c>
       <c r="C14" s="113" t="s">
@@ -13433,8 +14101,8 @@
       <c r="L14" s="112"/>
     </row>
     <row r="15" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="162"/>
-      <c r="B15" s="171"/>
+      <c r="A15" s="179"/>
+      <c r="B15" s="188"/>
       <c r="C15" s="113" t="s">
         <v>179</v>
       </c>
@@ -13449,8 +14117,8 @@
       <c r="L15" s="112"/>
     </row>
     <row r="16" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="162"/>
-      <c r="B16" s="172"/>
+      <c r="A16" s="179"/>
+      <c r="B16" s="189"/>
       <c r="C16" s="113" t="s">
         <v>68</v>
       </c>
@@ -13465,8 +14133,8 @@
       <c r="L16" s="112"/>
     </row>
     <row r="17" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="162"/>
-      <c r="B17" s="164" t="s">
+      <c r="A17" s="179"/>
+      <c r="B17" s="181" t="s">
         <v>159</v>
       </c>
       <c r="C17" s="113" t="s">
@@ -13483,8 +14151,8 @@
       <c r="L17" s="112"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="163"/>
-      <c r="B18" s="165"/>
+      <c r="A18" s="180"/>
+      <c r="B18" s="182"/>
       <c r="C18" s="115" t="s">
         <v>161</v>
       </c>
@@ -13538,10 +14206,10 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="173" t="s">
+      <c r="A2" s="190" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="175" t="s">
+      <c r="B2" s="192" t="s">
         <v>50</v>
       </c>
       <c r="C2" s="24" t="s">
@@ -13558,16 +14226,16 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="174"/>
-      <c r="B3" s="176"/>
+      <c r="A3" s="191"/>
+      <c r="B3" s="193"/>
       <c r="C3" s="40"/>
       <c r="D3" s="41"/>
       <c r="E3" s="41"/>
       <c r="F3" s="42"/>
     </row>
     <row r="4" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="174"/>
-      <c r="B4" s="176" t="s">
+      <c r="A4" s="191"/>
+      <c r="B4" s="193" t="s">
         <v>51</v>
       </c>
       <c r="C4" s="30" t="s">
@@ -13584,8 +14252,8 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="174"/>
-      <c r="B5" s="176"/>
+      <c r="A5" s="191"/>
+      <c r="B5" s="193"/>
       <c r="C5" s="34" t="s">
         <v>54</v>
       </c>
@@ -13594,10 +14262,10 @@
       <c r="F5" s="29"/>
     </row>
     <row r="6" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="174" t="s">
+      <c r="A6" s="191" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="176" t="s">
+      <c r="B6" s="193" t="s">
         <v>50</v>
       </c>
       <c r="C6" s="30" t="s">
@@ -13612,16 +14280,16 @@
       <c r="F6" s="29"/>
     </row>
     <row r="7" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="174"/>
-      <c r="B7" s="176"/>
+      <c r="A7" s="191"/>
+      <c r="B7" s="193"/>
       <c r="C7" s="40"/>
       <c r="D7" s="41"/>
       <c r="E7" s="41"/>
       <c r="F7" s="42"/>
     </row>
     <row r="8" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="174"/>
-      <c r="B8" s="176" t="s">
+      <c r="A8" s="191"/>
+      <c r="B8" s="193" t="s">
         <v>51</v>
       </c>
       <c r="C8" s="30" t="s">
@@ -13636,8 +14304,8 @@
       <c r="F8" s="29"/>
     </row>
     <row r="9" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="177"/>
-      <c r="B9" s="178"/>
+      <c r="A9" s="194"/>
+      <c r="B9" s="195"/>
       <c r="C9" s="37" t="s">
         <v>54</v>
       </c>
@@ -13679,13 +14347,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="B2" s="181" t="s">
+      <c r="B2" s="198" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="182"/>
-      <c r="D2" s="182"/>
-      <c r="E2" s="182"/>
-      <c r="F2" s="183"/>
+      <c r="C2" s="199"/>
+      <c r="D2" s="199"/>
+      <c r="E2" s="199"/>
+      <c r="F2" s="200"/>
     </row>
     <row r="3" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="53" t="s">
@@ -13767,10 +14435,10 @@
       <c r="F9" s="73"/>
     </row>
     <row r="10" spans="2:6" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="B10" s="179" t="s">
+      <c r="B10" s="196" t="s">
         <v>94</v>
       </c>
-      <c r="C10" s="180"/>
+      <c r="C10" s="197"/>
       <c r="D10" s="65"/>
       <c r="E10" s="83"/>
       <c r="F10" s="73"/>
@@ -13872,8 +14540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ABC9983-6AED-4B25-8AB6-C5125DB391F9}">
   <dimension ref="B1:G17"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -13889,10 +14557,10 @@
   <sheetData>
     <row r="1" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:7" ht="150.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="184" t="s">
+      <c r="B2" s="201" t="s">
         <v>150</v>
       </c>
-      <c r="C2" s="186" t="s">
+      <c r="C2" s="203" t="s">
         <v>151</v>
       </c>
       <c r="D2" s="119" t="s">
@@ -13905,8 +14573,8 @@
       <c r="G2" s="122"/>
     </row>
     <row r="3" spans="2:7" ht="176.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="185"/>
-      <c r="C3" s="187"/>
+      <c r="B3" s="202"/>
+      <c r="C3" s="204"/>
       <c r="D3" s="123" t="s">
         <v>153</v>
       </c>
@@ -13917,14 +14585,14 @@
       <c r="G3" s="125"/>
     </row>
     <row r="4" spans="2:7" ht="191.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="199" t="s">
+      <c r="B4" s="216" t="s">
         <v>123</v>
       </c>
-      <c r="C4" s="188" t="s">
+      <c r="C4" s="205" t="s">
         <v>127</v>
       </c>
-      <c r="D4" s="188"/>
-      <c r="E4" s="197" t="s">
+      <c r="D4" s="205"/>
+      <c r="E4" s="214" t="s">
         <v>139</v>
       </c>
       <c r="F4" s="99" t="s">
@@ -13935,10 +14603,10 @@
       </c>
     </row>
     <row r="5" spans="2:7" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="200"/>
-      <c r="C5" s="189"/>
-      <c r="D5" s="189"/>
-      <c r="E5" s="198"/>
+      <c r="B5" s="217"/>
+      <c r="C5" s="206"/>
+      <c r="D5" s="206"/>
+      <c r="E5" s="215"/>
       <c r="F5" s="102" t="s">
         <v>129</v>
       </c>
@@ -13947,8 +14615,8 @@
       </c>
     </row>
     <row r="6" spans="2:7" ht="79.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="200"/>
-      <c r="C6" s="189" t="s">
+      <c r="B6" s="217"/>
+      <c r="C6" s="206" t="s">
         <v>124</v>
       </c>
       <c r="D6" s="102" t="s">
@@ -13961,8 +14629,8 @@
       <c r="G6" s="128"/>
     </row>
     <row r="7" spans="2:7" ht="155.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="200"/>
-      <c r="C7" s="189"/>
+      <c r="B7" s="217"/>
+      <c r="C7" s="206"/>
       <c r="D7" s="101" t="s">
         <v>156</v>
       </c>
@@ -13973,12 +14641,12 @@
       <c r="G7" s="104"/>
     </row>
     <row r="8" spans="2:7" ht="99.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="200"/>
-      <c r="C8" s="189"/>
-      <c r="D8" s="194" t="s">
+      <c r="B8" s="217"/>
+      <c r="C8" s="206"/>
+      <c r="D8" s="211" t="s">
         <v>152</v>
       </c>
-      <c r="E8" s="191" t="s">
+      <c r="E8" s="208" t="s">
         <v>126</v>
       </c>
       <c r="F8" s="101" t="s">
@@ -13989,10 +14657,10 @@
       </c>
     </row>
     <row r="9" spans="2:7" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="200"/>
-      <c r="C9" s="189"/>
-      <c r="D9" s="195"/>
-      <c r="E9" s="192"/>
+      <c r="B9" s="217"/>
+      <c r="C9" s="206"/>
+      <c r="D9" s="212"/>
+      <c r="E9" s="209"/>
       <c r="F9" s="101" t="s">
         <v>148</v>
       </c>
@@ -14001,10 +14669,10 @@
       </c>
     </row>
     <row r="10" spans="2:7" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="200"/>
-      <c r="C10" s="189"/>
-      <c r="D10" s="195"/>
-      <c r="E10" s="192"/>
+      <c r="B10" s="217"/>
+      <c r="C10" s="206"/>
+      <c r="D10" s="212"/>
+      <c r="E10" s="209"/>
       <c r="F10" s="101" t="s">
         <v>137</v>
       </c>
@@ -14013,10 +14681,10 @@
       </c>
     </row>
     <row r="11" spans="2:7" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="200"/>
-      <c r="C11" s="189"/>
-      <c r="D11" s="195"/>
-      <c r="E11" s="192"/>
+      <c r="B11" s="217"/>
+      <c r="C11" s="206"/>
+      <c r="D11" s="212"/>
+      <c r="E11" s="209"/>
       <c r="F11" s="101" t="s">
         <v>136</v>
       </c>
@@ -14025,10 +14693,10 @@
       </c>
     </row>
     <row r="12" spans="2:7" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="200"/>
-      <c r="C12" s="189"/>
-      <c r="D12" s="195"/>
-      <c r="E12" s="192"/>
+      <c r="B12" s="217"/>
+      <c r="C12" s="206"/>
+      <c r="D12" s="212"/>
+      <c r="E12" s="209"/>
       <c r="F12" s="101" t="s">
         <v>135</v>
       </c>
@@ -14037,10 +14705,10 @@
       </c>
     </row>
     <row r="13" spans="2:7" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="201"/>
-      <c r="C13" s="190"/>
-      <c r="D13" s="196"/>
-      <c r="E13" s="193"/>
+      <c r="B13" s="218"/>
+      <c r="C13" s="207"/>
+      <c r="D13" s="213"/>
+      <c r="E13" s="210"/>
       <c r="F13" s="105" t="s">
         <v>133</v>
       </c>
@@ -14069,276 +14737,448 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{170671FC-7126-4F53-9577-31F7E194AC02}">
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9:D15"/>
+    <sheetView topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="101" style="202" customWidth="1"/>
-    <col min="2" max="2" width="12.75" style="202" customWidth="1"/>
-    <col min="3" max="3" width="74.75" style="202" customWidth="1"/>
-    <col min="4" max="4" width="84.625" style="202" customWidth="1"/>
-    <col min="5" max="5" width="41.375" style="202" customWidth="1"/>
-    <col min="6" max="6" width="33.75" style="204" customWidth="1"/>
-    <col min="7" max="7" width="43.125" style="203" customWidth="1"/>
-    <col min="8" max="8" width="46.375" style="203" customWidth="1"/>
-    <col min="9" max="9" width="27.25" style="203" customWidth="1"/>
-    <col min="10" max="10" width="16.125" style="203" customWidth="1"/>
-    <col min="11" max="11" width="14" style="203" customWidth="1"/>
-    <col min="12" max="12" width="53.375" style="203" customWidth="1"/>
+    <col min="1" max="1" width="57.625" style="138" customWidth="1"/>
+    <col min="2" max="2" width="12.75" style="138" customWidth="1"/>
+    <col min="3" max="3" width="68.375" style="138" customWidth="1"/>
+    <col min="4" max="4" width="84.625" style="138" customWidth="1"/>
+    <col min="5" max="5" width="42.25" style="138" customWidth="1"/>
+    <col min="6" max="6" width="69" style="140" customWidth="1"/>
+    <col min="7" max="7" width="41.5" style="139" customWidth="1"/>
+    <col min="8" max="8" width="44.625" style="139" customWidth="1"/>
+    <col min="9" max="9" width="43.5" style="139" customWidth="1"/>
+    <col min="10" max="10" width="41.625" style="139" customWidth="1"/>
+    <col min="11" max="11" width="37.5" style="139" customWidth="1"/>
+    <col min="12" max="12" width="56.25" style="139" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="203" t="s">
-        <v>200</v>
-      </c>
-      <c r="B1" s="203"/>
-      <c r="C1" s="203"/>
+      <c r="A1" s="139" t="s">
+        <v>230</v>
+      </c>
+      <c r="B1" s="139"/>
+      <c r="C1" s="139"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="203" t="s">
-        <v>199</v>
-      </c>
-      <c r="B2" s="203"/>
-      <c r="C2" s="203"/>
+      <c r="A2" s="139" t="s">
+        <v>194</v>
+      </c>
+      <c r="B2" s="139"/>
+      <c r="C2" s="139"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="203" t="s">
-        <v>198</v>
-      </c>
-      <c r="B3" s="203"/>
-      <c r="C3" s="203"/>
+      <c r="A3" s="139" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" s="139"/>
+      <c r="C3" s="139"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="203" t="s">
-        <v>77</v>
-      </c>
-      <c r="B4" s="203"/>
-      <c r="C4" s="203"/>
+      <c r="A4" s="219" t="s">
+        <v>110</v>
+      </c>
+      <c r="B4" s="220" t="s">
+        <v>216</v>
+      </c>
+      <c r="C4" s="229" t="s">
+        <v>217</v>
+      </c>
+      <c r="D4" s="141" t="s">
+        <v>218</v>
+      </c>
+      <c r="E4" s="150" t="s">
+        <v>221</v>
+      </c>
+      <c r="F4" s="151"/>
+      <c r="G4" s="141"/>
+      <c r="H4" s="143"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="206" t="s">
-        <v>110</v>
-      </c>
-      <c r="B5" s="205" t="s">
+      <c r="A5" s="219"/>
+      <c r="B5" s="220"/>
+      <c r="C5" s="230"/>
+      <c r="D5" s="147" t="s">
+        <v>219</v>
+      </c>
+      <c r="E5" s="152" t="s">
         <v>222</v>
       </c>
-      <c r="C5" s="227" t="s">
+      <c r="F5" s="153" t="s">
         <v>223</v>
       </c>
-      <c r="D5" s="228" t="s">
+      <c r="G5" s="147" t="s">
         <v>224</v>
       </c>
-      <c r="E5" s="231" t="s">
-        <v>227</v>
-      </c>
-      <c r="F5" s="232"/>
-      <c r="G5" s="233"/>
-      <c r="H5" s="234"/>
+      <c r="H5" s="154" t="s">
+        <v>225</v>
+      </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="206"/>
-      <c r="B6" s="205"/>
-      <c r="C6" s="229"/>
-      <c r="D6" s="230" t="s">
-        <v>225</v>
-      </c>
-      <c r="E6" s="235" t="s">
+    <row r="6" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="219"/>
+      <c r="B6" s="219" t="s">
+        <v>193</v>
+      </c>
+      <c r="C6" s="223" t="s">
+        <v>226</v>
+      </c>
+      <c r="D6" s="223" t="s">
         <v>228</v>
       </c>
-      <c r="F6" s="236" t="s">
-        <v>229</v>
-      </c>
-      <c r="G6" s="237" t="s">
-        <v>230</v>
-      </c>
-      <c r="H6" s="238" t="s">
-        <v>231</v>
-      </c>
+      <c r="E6" s="223" t="s">
+        <v>209</v>
+      </c>
+      <c r="F6" s="221" t="s">
+        <v>202</v>
+      </c>
+      <c r="G6" s="141" t="s">
+        <v>203</v>
+      </c>
+      <c r="H6" s="142" t="s">
+        <v>195</v>
+      </c>
+      <c r="I6" s="141"/>
+      <c r="J6" s="141"/>
+      <c r="K6" s="141"/>
+      <c r="L6" s="143"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="206"/>
-      <c r="B7" s="206" t="s">
-        <v>193</v>
-      </c>
-      <c r="C7" s="203" t="s">
-        <v>194</v>
-      </c>
-      <c r="D7" s="203"/>
+    <row r="7" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="219"/>
+      <c r="B7" s="219"/>
+      <c r="C7" s="223"/>
+      <c r="D7" s="223"/>
+      <c r="E7" s="223"/>
+      <c r="F7" s="222"/>
+      <c r="G7" s="224" t="s">
+        <v>204</v>
+      </c>
+      <c r="H7" s="224" t="s">
+        <v>220</v>
+      </c>
+      <c r="I7" s="225" t="s">
+        <v>205</v>
+      </c>
+      <c r="J7" s="224" t="s">
+        <v>196</v>
+      </c>
+      <c r="K7" s="144" t="s">
+        <v>206</v>
+      </c>
+      <c r="L7" s="145" t="s">
+        <v>198</v>
+      </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="206"/>
-      <c r="B8" s="206"/>
-      <c r="C8" s="203" t="s">
-        <v>195</v>
-      </c>
-      <c r="D8" s="203"/>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" s="219"/>
+      <c r="B8" s="219"/>
+      <c r="C8" s="223"/>
+      <c r="D8" s="223"/>
+      <c r="E8" s="223"/>
+      <c r="F8" s="222"/>
+      <c r="G8" s="224"/>
+      <c r="H8" s="224"/>
+      <c r="I8" s="225"/>
+      <c r="J8" s="224"/>
+      <c r="K8" s="144" t="s">
+        <v>207</v>
+      </c>
+      <c r="L8" s="146" t="s">
+        <v>199</v>
+      </c>
     </row>
-    <row r="9" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="206"/>
-      <c r="B9" s="206"/>
-      <c r="C9" s="206" t="s">
-        <v>196</v>
-      </c>
-      <c r="D9" s="207" t="s">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" s="219"/>
+      <c r="B9" s="219"/>
+      <c r="C9" s="223"/>
+      <c r="D9" s="223"/>
+      <c r="E9" s="223"/>
+      <c r="F9" s="222"/>
+      <c r="G9" s="224"/>
+      <c r="H9" s="224"/>
+      <c r="I9" s="225"/>
+      <c r="J9" s="144" t="s">
         <v>197</v>
       </c>
-      <c r="E9" s="207" t="s">
+      <c r="K9" s="144"/>
+      <c r="L9" s="146" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" s="219"/>
+      <c r="B10" s="219"/>
+      <c r="C10" s="223"/>
+      <c r="D10" s="223"/>
+      <c r="E10" s="223"/>
+      <c r="F10" s="222"/>
+      <c r="G10" s="224"/>
+      <c r="H10" s="226" t="s">
+        <v>208</v>
+      </c>
+      <c r="I10" s="226" t="s">
+        <v>210</v>
+      </c>
+      <c r="J10" s="232"/>
+      <c r="K10" s="144" t="s">
+        <v>212</v>
+      </c>
+      <c r="L10" s="145" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="219"/>
+      <c r="B11" s="219"/>
+      <c r="C11" s="223"/>
+      <c r="D11" s="223"/>
+      <c r="E11" s="223"/>
+      <c r="F11" s="222"/>
+      <c r="G11" s="224"/>
+      <c r="H11" s="227"/>
+      <c r="I11" s="228"/>
+      <c r="J11" s="233"/>
+      <c r="K11" s="144" t="s">
+        <v>214</v>
+      </c>
+      <c r="L11" s="149" t="s">
         <v>215</v>
-      </c>
-      <c r="F9" s="208" t="s">
-        <v>208</v>
-      </c>
-      <c r="G9" s="209" t="s">
-        <v>209</v>
-      </c>
-      <c r="H9" s="210" t="s">
-        <v>201</v>
-      </c>
-      <c r="I9" s="209"/>
-      <c r="J9" s="209"/>
-      <c r="K9" s="209"/>
-      <c r="L9" s="211"/>
-    </row>
-    <row r="10" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="206"/>
-      <c r="B10" s="206"/>
-      <c r="C10" s="206"/>
-      <c r="D10" s="207"/>
-      <c r="E10" s="207"/>
-      <c r="F10" s="212"/>
-      <c r="G10" s="213" t="s">
-        <v>210</v>
-      </c>
-      <c r="H10" s="213" t="s">
-        <v>226</v>
-      </c>
-      <c r="I10" s="214" t="s">
-        <v>211</v>
-      </c>
-      <c r="J10" s="213" t="s">
-        <v>202</v>
-      </c>
-      <c r="K10" s="215" t="s">
-        <v>212</v>
-      </c>
-      <c r="L10" s="216" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" s="206"/>
-      <c r="B11" s="206"/>
-      <c r="C11" s="206"/>
-      <c r="D11" s="207"/>
-      <c r="E11" s="207"/>
-      <c r="F11" s="212"/>
-      <c r="G11" s="213"/>
-      <c r="H11" s="213"/>
-      <c r="I11" s="214"/>
-      <c r="J11" s="213"/>
-      <c r="K11" s="215" t="s">
-        <v>213</v>
-      </c>
-      <c r="L11" s="217" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" s="206"/>
-      <c r="B12" s="206"/>
-      <c r="C12" s="206"/>
-      <c r="D12" s="207"/>
-      <c r="E12" s="207"/>
-      <c r="F12" s="212"/>
-      <c r="G12" s="213"/>
-      <c r="H12" s="213"/>
-      <c r="I12" s="214"/>
-      <c r="J12" s="215" t="s">
-        <v>203</v>
-      </c>
-      <c r="K12" s="215"/>
-      <c r="L12" s="217" t="s">
-        <v>206</v>
+      <c r="A12" s="219"/>
+      <c r="B12" s="219"/>
+      <c r="C12" s="223"/>
+      <c r="D12" s="223"/>
+      <c r="E12" s="223"/>
+      <c r="F12" s="234"/>
+      <c r="G12" s="226"/>
+      <c r="H12" s="227"/>
+      <c r="I12" s="148" t="s">
+        <v>211</v>
+      </c>
+      <c r="J12" s="233"/>
+      <c r="K12" s="148"/>
+      <c r="L12" s="235" t="s">
+        <v>201</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="206"/>
-      <c r="B13" s="206"/>
-      <c r="C13" s="206"/>
-      <c r="D13" s="207"/>
-      <c r="E13" s="207"/>
-      <c r="F13" s="212"/>
-      <c r="G13" s="213"/>
-      <c r="H13" s="222" t="s">
-        <v>214</v>
-      </c>
-      <c r="I13" s="222" t="s">
-        <v>216</v>
-      </c>
-      <c r="J13" s="215"/>
-      <c r="K13" s="215" t="s">
-        <v>218</v>
-      </c>
-      <c r="L13" s="216" t="s">
-        <v>219</v>
-      </c>
+    <row r="13" spans="1:12" ht="82.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="219"/>
+      <c r="B13" s="219"/>
+      <c r="C13" s="223" t="s">
+        <v>227</v>
+      </c>
+      <c r="D13" s="236" t="s">
+        <v>229</v>
+      </c>
+      <c r="E13" s="237" t="s">
+        <v>236</v>
+      </c>
+      <c r="F13" s="237" t="s">
+        <v>233</v>
+      </c>
+      <c r="G13" s="237" t="s">
+        <v>232</v>
+      </c>
+      <c r="H13" s="237" t="s">
+        <v>234</v>
+      </c>
+      <c r="I13" s="238" t="s">
+        <v>238</v>
+      </c>
+      <c r="J13" s="239"/>
+      <c r="K13" s="239"/>
+      <c r="L13" s="240"/>
     </row>
-    <row r="14" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="206"/>
-      <c r="B14" s="206"/>
-      <c r="C14" s="206"/>
-      <c r="D14" s="207"/>
-      <c r="E14" s="207"/>
-      <c r="F14" s="212"/>
-      <c r="G14" s="213"/>
-      <c r="H14" s="223"/>
-      <c r="I14" s="225"/>
-      <c r="J14" s="215"/>
-      <c r="K14" s="215" t="s">
-        <v>220</v>
-      </c>
-      <c r="L14" s="226" t="s">
-        <v>221</v>
+    <row r="14" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="219"/>
+      <c r="B14" s="219"/>
+      <c r="C14" s="223"/>
+      <c r="D14" s="241"/>
+      <c r="E14" s="242"/>
+      <c r="F14" s="242"/>
+      <c r="G14" s="242"/>
+      <c r="H14" s="242"/>
+      <c r="I14" s="242" t="s">
+        <v>235</v>
+      </c>
+      <c r="J14" s="242" t="s">
+        <v>239</v>
+      </c>
+      <c r="K14" s="242" t="s">
+        <v>244</v>
+      </c>
+      <c r="L14" s="243" t="s">
+        <v>245</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="206"/>
-      <c r="B15" s="206"/>
-      <c r="C15" s="206"/>
-      <c r="D15" s="207"/>
-      <c r="E15" s="207"/>
-      <c r="F15" s="218"/>
-      <c r="G15" s="219"/>
-      <c r="H15" s="224"/>
-      <c r="I15" s="220" t="s">
-        <v>217</v>
-      </c>
-      <c r="J15" s="220"/>
-      <c r="K15" s="220"/>
-      <c r="L15" s="221" t="s">
-        <v>207</v>
-      </c>
+    <row r="15" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="219"/>
+      <c r="B15" s="219"/>
+      <c r="C15" s="223"/>
+      <c r="D15" s="241"/>
+      <c r="E15" s="242"/>
+      <c r="F15" s="242"/>
+      <c r="G15" s="242"/>
+      <c r="H15" s="242"/>
+      <c r="I15" s="242"/>
+      <c r="J15" s="242"/>
+      <c r="K15" s="242"/>
+      <c r="L15" s="243"/>
+    </row>
+    <row r="16" spans="1:12" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="219"/>
+      <c r="B16" s="219"/>
+      <c r="C16" s="223"/>
+      <c r="D16" s="241"/>
+      <c r="E16" s="242"/>
+      <c r="F16" s="242"/>
+      <c r="G16" s="242"/>
+      <c r="H16" s="242"/>
+      <c r="I16" s="242"/>
+      <c r="J16" s="242" t="s">
+        <v>240</v>
+      </c>
+      <c r="K16" s="242"/>
+      <c r="L16" s="244" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="219"/>
+      <c r="B17" s="219"/>
+      <c r="C17" s="223"/>
+      <c r="D17" s="241"/>
+      <c r="E17" s="242"/>
+      <c r="F17" s="242"/>
+      <c r="G17" s="242"/>
+      <c r="H17" s="242"/>
+      <c r="I17" s="242"/>
+      <c r="J17" s="242"/>
+      <c r="K17" s="242"/>
+      <c r="L17" s="244"/>
+    </row>
+    <row r="18" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="219"/>
+      <c r="B18" s="219"/>
+      <c r="C18" s="223"/>
+      <c r="D18" s="241"/>
+      <c r="E18" s="242" t="s">
+        <v>237</v>
+      </c>
+      <c r="F18" s="245" t="s">
+        <v>249</v>
+      </c>
+      <c r="G18" s="242" t="s">
+        <v>231</v>
+      </c>
+      <c r="H18" s="242"/>
+      <c r="I18" s="245" t="s">
+        <v>247</v>
+      </c>
+      <c r="J18" s="242" t="s">
+        <v>241</v>
+      </c>
+      <c r="K18" s="242" t="s">
+        <v>243</v>
+      </c>
+      <c r="L18" s="246" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="219"/>
+      <c r="B19" s="219"/>
+      <c r="C19" s="223"/>
+      <c r="D19" s="241"/>
+      <c r="E19" s="242"/>
+      <c r="F19" s="245"/>
+      <c r="G19" s="242"/>
+      <c r="H19" s="242"/>
+      <c r="I19" s="245"/>
+      <c r="J19" s="242"/>
+      <c r="K19" s="242"/>
+      <c r="L19" s="246"/>
+    </row>
+    <row r="20" spans="1:12" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="219"/>
+      <c r="B20" s="219"/>
+      <c r="C20" s="223"/>
+      <c r="D20" s="241"/>
+      <c r="E20" s="242"/>
+      <c r="F20" s="245"/>
+      <c r="G20" s="242"/>
+      <c r="H20" s="242"/>
+      <c r="I20" s="245"/>
+      <c r="J20" s="242" t="s">
+        <v>242</v>
+      </c>
+      <c r="K20" s="242"/>
+      <c r="L20" s="244" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="219"/>
+      <c r="B21" s="219"/>
+      <c r="C21" s="223"/>
+      <c r="D21" s="247"/>
+      <c r="E21" s="248"/>
+      <c r="F21" s="249"/>
+      <c r="G21" s="248"/>
+      <c r="H21" s="248"/>
+      <c r="I21" s="249"/>
+      <c r="J21" s="248"/>
+      <c r="K21" s="248"/>
+      <c r="L21" s="250"/>
+    </row>
+    <row r="25" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C25" s="231"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="B7:B15"/>
-    <mergeCell ref="A5:A15"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="F9:F15"/>
-    <mergeCell ref="E9:E15"/>
-    <mergeCell ref="D9:D15"/>
-    <mergeCell ref="C9:C15"/>
-    <mergeCell ref="G10:G15"/>
-    <mergeCell ref="J10:J11"/>
+  <mergeCells count="36">
+    <mergeCell ref="L16:L17"/>
+    <mergeCell ref="L14:L15"/>
+    <mergeCell ref="J18:J19"/>
+    <mergeCell ref="J20:J21"/>
+    <mergeCell ref="K18:K21"/>
+    <mergeCell ref="L18:L19"/>
+    <mergeCell ref="L20:L21"/>
+    <mergeCell ref="H13:H21"/>
+    <mergeCell ref="I18:I21"/>
+    <mergeCell ref="K14:K17"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="I14:I17"/>
+    <mergeCell ref="J10:J12"/>
+    <mergeCell ref="G13:G17"/>
+    <mergeCell ref="F13:F17"/>
+    <mergeCell ref="E13:E17"/>
+    <mergeCell ref="G18:G21"/>
+    <mergeCell ref="F18:F21"/>
+    <mergeCell ref="E18:E21"/>
+    <mergeCell ref="C6:C12"/>
+    <mergeCell ref="D13:D21"/>
+    <mergeCell ref="C13:C21"/>
+    <mergeCell ref="G7:G12"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="H7:H9"/>
+    <mergeCell ref="I7:I9"/>
     <mergeCell ref="H10:H12"/>
-    <mergeCell ref="I10:I12"/>
-    <mergeCell ref="H13:H15"/>
-    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="I10:I11"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="F6:F12"/>
+    <mergeCell ref="E6:E12"/>
+    <mergeCell ref="D6:D12"/>
+    <mergeCell ref="B6:B21"/>
+    <mergeCell ref="A4:A21"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>